<commit_message>
swapped lox and fuel tanks to reflect sizing. started pv combined load analysis
</commit_message>
<xml_diff>
--- a/vehicle-sims/thickness-weight-study/matrix.xlsx
+++ b/vehicle-sims/thickness-weight-study/matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_repos\upstream-salmon-rocket\vehicle-sims\thickness-weight-study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2019CF37-C709-4967-BC8F-1615C6F1AF29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A506DF76-170E-4380-9B8E-7018F0D91E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38010" yWindow="390" windowWidth="28800" windowHeight="17355" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="59">
   <si>
     <t>Original Size</t>
   </si>
@@ -193,6 +193,24 @@
   </si>
   <si>
     <t>m s^-1 $^-1</t>
+  </si>
+  <si>
+    <t>Hoop stress</t>
+  </si>
+  <si>
+    <t>Axial stress</t>
+  </si>
+  <si>
+    <t>Estimate worst compression</t>
+  </si>
+  <si>
+    <t>von Mises combined stress</t>
+  </si>
+  <si>
+    <t>6061-T6 Yeild</t>
+  </si>
+  <si>
+    <t>FOS</t>
   </si>
 </sst>
 </file>
@@ -225,7 +243,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -235,6 +253,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -266,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -280,6 +304,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -560,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L54"/>
+  <dimension ref="A1:N54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,7 +617,7 @@
       <c r="F1" t="s">
         <v>41</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="11" t="s">
         <v>42</v>
       </c>
       <c r="H1" t="s">
@@ -621,7 +646,7 @@
       <c r="F2">
         <v>2</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="11">
         <v>2</v>
       </c>
       <c r="H2">
@@ -656,7 +681,7 @@
       <c r="F3">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="11">
         <v>4.9000000000000002E-2</v>
       </c>
       <c r="H3">
@@ -695,7 +720,7 @@
         <f t="shared" si="0"/>
         <v>1.87</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="11">
         <f t="shared" si="0"/>
         <v>1.9019999999999999</v>
       </c>
@@ -716,11 +741,15 @@
         <v>2.87</v>
       </c>
     </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G5" s="11"/>
+    </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1"/>
+      <c r="G6" s="11"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -741,7 +770,7 @@
       <c r="F7">
         <v>6</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="11">
         <v>6</v>
       </c>
       <c r="H7">
@@ -776,7 +805,7 @@
       <c r="F8">
         <v>12</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="11">
         <v>12</v>
       </c>
       <c r="H8">
@@ -811,7 +840,7 @@
       <c r="F9">
         <v>18</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="11">
         <v>18</v>
       </c>
       <c r="H9">
@@ -846,7 +875,7 @@
       <c r="F10">
         <v>16</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="11">
         <v>16</v>
       </c>
       <c r="H10">
@@ -881,7 +910,7 @@
       <c r="F11">
         <v>10</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="11">
         <v>10</v>
       </c>
       <c r="H11">
@@ -916,7 +945,7 @@
       <c r="F12">
         <v>9</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="11">
         <v>9</v>
       </c>
       <c r="H12">
@@ -955,7 +984,7 @@
         <f t="shared" si="3"/>
         <v>71</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="11">
         <f t="shared" si="3"/>
         <v>71</v>
       </c>
@@ -1500,39 +1529,39 @@
         <v>29</v>
       </c>
       <c r="C34" s="4">
-        <f>C33*C13</f>
+        <f t="shared" ref="C34:K34" si="10">C33*C13</f>
         <v>53.960625</v>
       </c>
       <c r="D34" s="4">
-        <f>D33*D13</f>
+        <f t="shared" si="10"/>
         <v>47.298819444444447</v>
       </c>
       <c r="E34" s="4">
-        <f>E33*E13</f>
+        <f t="shared" si="10"/>
         <v>28.181083333333337</v>
       </c>
       <c r="F34" s="4">
-        <f>F33*F13</f>
+        <f t="shared" si="10"/>
         <v>98.931597222222223</v>
       </c>
       <c r="G34" s="4">
-        <f>G33*G13</f>
+        <f t="shared" si="10"/>
         <v>75.183576388888895</v>
       </c>
       <c r="H34" s="4">
-        <f>H33*H13</f>
+        <f t="shared" si="10"/>
         <v>43.091145833333336</v>
       </c>
       <c r="I34" s="4">
-        <f>I33*I13</f>
+        <f t="shared" si="10"/>
         <v>141.63020833333334</v>
       </c>
       <c r="J34" s="4">
-        <f>J33*J13</f>
+        <f t="shared" si="10"/>
         <v>36.196562499999999</v>
       </c>
       <c r="K34" s="4">
-        <f>K33*K13</f>
+        <f t="shared" si="10"/>
         <v>118.969375</v>
       </c>
     </row>
@@ -1579,39 +1608,39 @@
         <v>34</v>
       </c>
       <c r="C37" s="5">
-        <f>C36*(C9/(C9+C10+C11))</f>
+        <f t="shared" ref="C37:K37" si="11">C36*(C9/(C9+C10+C11))</f>
         <v>444.4444444444444</v>
       </c>
       <c r="D37" s="5">
-        <f>D36*(D9/(D9+D10+D11))</f>
+        <f t="shared" si="11"/>
         <v>409.09090909090912</v>
       </c>
       <c r="E37" s="5">
-        <f>E36*(E9/(E9+E10+E11))</f>
+        <f t="shared" si="11"/>
         <v>409.09090909090912</v>
       </c>
       <c r="F37" s="5">
-        <f>F36*(F9/(F9+F10+F11))</f>
+        <f t="shared" si="11"/>
         <v>409.09090909090912</v>
       </c>
       <c r="G37" s="5">
-        <f>G36*(G9/(G9+G10+G11))</f>
+        <f t="shared" si="11"/>
         <v>409.09090909090912</v>
       </c>
       <c r="H37" s="5">
-        <f>H36*(H9/(H9+H10+H11))</f>
+        <f t="shared" si="11"/>
         <v>409.09090909090912</v>
       </c>
       <c r="I37" s="5">
-        <f>I36*(I9/(I9+I10+I11))</f>
+        <f t="shared" si="11"/>
         <v>409.09090909090912</v>
       </c>
       <c r="J37" s="5">
-        <f>J36*(J9/(J9+J10+J11))</f>
+        <f t="shared" si="11"/>
         <v>406.25</v>
       </c>
       <c r="K37" s="5">
-        <f>K36*(K9/(K9+K10+K11))</f>
+        <f t="shared" si="11"/>
         <v>406.25</v>
       </c>
     </row>
@@ -1623,39 +1652,39 @@
         <v>23</v>
       </c>
       <c r="C39" s="4">
-        <f>C20/C21</f>
+        <f t="shared" ref="C39:K39" si="12">C20/C21</f>
         <v>1.2829324169530354</v>
       </c>
       <c r="D39" s="4">
-        <f>D20/D21</f>
+        <f t="shared" si="12"/>
         <v>1.285892634207241</v>
       </c>
       <c r="E39" s="4">
-        <f>E20/E21</f>
+        <f t="shared" si="12"/>
         <v>1.2636363636363637</v>
       </c>
       <c r="F39" s="4">
-        <f>F20/F21</f>
+        <f t="shared" si="12"/>
         <v>1.3804878048780487</v>
       </c>
       <c r="G39" s="4">
-        <f>G20/G21</f>
+        <f t="shared" si="12"/>
         <v>1.4298401420959148</v>
       </c>
       <c r="H39" s="4">
-        <f>H20/H21</f>
+        <f t="shared" si="12"/>
         <v>1.3722627737226278</v>
       </c>
       <c r="I39" s="4">
-        <f>I20/I21</f>
+        <f t="shared" si="12"/>
         <v>1.5092592592592593</v>
       </c>
       <c r="J39" s="4">
-        <f>J20/J21</f>
+        <f t="shared" si="12"/>
         <v>1.282258064516129</v>
       </c>
       <c r="K39" s="4">
-        <f>K20/K21</f>
+        <f t="shared" si="12"/>
         <v>1.3762376237623763</v>
       </c>
     </row>
@@ -1671,35 +1700,35 @@
         <v>0.24914840844953792</v>
       </c>
       <c r="D40" s="4">
-        <f t="shared" ref="D40:K40" si="10">LN(D39)</f>
+        <f t="shared" ref="D40:K40" si="13">LN(D39)</f>
         <v>0.25145313415532228</v>
       </c>
       <c r="E40" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.23399356733827556</v>
       </c>
       <c r="F40" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.32243691850482936</v>
       </c>
       <c r="G40" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.35756264927887305</v>
       </c>
       <c r="H40" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.31646103700182437</v>
       </c>
       <c r="I40" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.41161897368254269</v>
       </c>
       <c r="J40" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.24862263661519463</v>
       </c>
       <c r="K40" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.31935341628943237</v>
       </c>
     </row>
@@ -1750,35 +1779,35 @@
         <v>548.1264985889834</v>
       </c>
       <c r="D43" s="5">
-        <f t="shared" ref="D43:K43" si="11">D40*D42</f>
+        <f t="shared" ref="D43:K43" si="14">D40*D42</f>
         <v>553.19689514170898</v>
       </c>
       <c r="E43" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>514.78584814420628</v>
       </c>
       <c r="F43" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>709.36122071062459</v>
       </c>
       <c r="G43" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>786.63782841352065</v>
       </c>
       <c r="H43" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>696.2142814040136</v>
       </c>
       <c r="I43" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>905.56174210159395</v>
       </c>
       <c r="J43" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>546.96980055342817</v>
       </c>
       <c r="K43" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>702.57751583675122</v>
       </c>
     </row>
@@ -1794,64 +1823,103 @@
         <v>10.157897514882071</v>
       </c>
       <c r="D44" s="6">
-        <f t="shared" ref="D44:K44" si="12">D43/D34</f>
+        <f t="shared" ref="D44:K44" si="15">D43/D34</f>
         <v>11.695786525739292</v>
       </c>
       <c r="E44" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>18.267070930353619</v>
       </c>
       <c r="F44" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>7.1702190263565901</v>
       </c>
       <c r="G44" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>10.46289450696808</v>
       </c>
       <c r="H44" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>16.156782743647863</v>
       </c>
       <c r="I44" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>6.3938460075573138</v>
       </c>
       <c r="J44" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>15.111097926866071</v>
       </c>
       <c r="K44" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>5.9055325442934468</v>
       </c>
     </row>
-    <row r="50" spans="10:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="51" spans="10:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J51" s="3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L51" s="3">
         <v>3.7509238730000001E-4</v>
       </c>
-      <c r="K51" t="s">
+      <c r="M51" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="52" spans="10:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J52" s="3">
+    <row r="52" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>57</v>
+      </c>
+      <c r="L52" s="3">
         <v>6.2000371819999995E-4</v>
       </c>
-      <c r="K52">
-        <f>J52/J51</f>
+      <c r="M52">
+        <f>L52/L51</f>
         <v>1.6529360210771731</v>
       </c>
     </row>
-    <row r="54" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="L54">
-        <f>7*K52</f>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N54">
+        <f>7*M52</f>
         <v>11.570552147540212</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C44:K44">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C43:K43">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1863,15 +1931,15 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C43:K43">
+  <conditionalFormatting sqref="C34:K34">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
intermediate sizing changes to thin walls
</commit_message>
<xml_diff>
--- a/vehicle-sims/thickness-weight-study/matrix.xlsx
+++ b/vehicle-sims/thickness-weight-study/matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_repos\upstream-salmon-rocket\vehicle-sims\thickness-weight-study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A506DF76-170E-4380-9B8E-7018F0D91E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E5A108D-734E-4FB0-A017-DFB71E0BCF7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38010" yWindow="390" windowWidth="28800" windowHeight="17355" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="17355" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="62">
   <si>
     <t>Original Size</t>
   </si>
@@ -120,9 +120,6 @@
     <t>Total Length</t>
   </si>
   <si>
-    <t>Tube cost per inch</t>
-  </si>
-  <si>
     <t>$</t>
   </si>
   <si>
@@ -207,10 +204,22 @@
     <t>von Mises combined stress</t>
   </si>
   <si>
-    <t>6061-T6 Yeild</t>
-  </si>
-  <si>
     <t>FOS</t>
+  </si>
+  <si>
+    <t>Thin Wall PV Estimation</t>
+  </si>
+  <si>
+    <t>6061-T6 Yeild*</t>
+  </si>
+  <si>
+    <t>Tube cost per inch (MWI)</t>
+  </si>
+  <si>
+    <t>Tube cost per inch (MCM)</t>
+  </si>
+  <si>
+    <t>* TYPICAL VALUE, CHECK LOT TENSILE TEST CERTIFICATE</t>
   </si>
 </sst>
 </file>
@@ -585,15 +594,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N54"/>
+  <dimension ref="A1:O57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.85546875" customWidth="1"/>
     <col min="4" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
@@ -609,22 +618,22 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
         <v>40</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" t="s">
         <v>42</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>43</v>
-      </c>
-      <c r="J1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1345,7 +1354,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B26" t="s">
         <v>22</v>
@@ -1439,15 +1448,15 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
         <v>31</v>
-      </c>
-      <c r="B31" t="s">
-        <v>32</v>
       </c>
       <c r="C31">
         <v>8.11</v>
@@ -1479,10 +1488,10 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="B33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C33" s="4">
         <f>191.86/288</f>
@@ -1523,391 +1532,533 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="B34" t="s">
         <v>29</v>
       </c>
-      <c r="C34" s="4">
-        <f t="shared" ref="C34:K34" si="10">C33*C13</f>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35" s="4">
+        <f>C33*C13</f>
         <v>53.960625</v>
       </c>
-      <c r="D34" s="4">
-        <f t="shared" si="10"/>
+      <c r="D35" s="4">
+        <f>D33*D13</f>
         <v>47.298819444444447</v>
       </c>
-      <c r="E34" s="4">
-        <f t="shared" si="10"/>
+      <c r="E35" s="4">
+        <f>E33*E13</f>
         <v>28.181083333333337</v>
       </c>
-      <c r="F34" s="4">
-        <f t="shared" si="10"/>
+      <c r="F35" s="4">
+        <f>F33*F13</f>
         <v>98.931597222222223</v>
       </c>
-      <c r="G34" s="4">
-        <f t="shared" si="10"/>
+      <c r="G35" s="4">
+        <f>G33*G13</f>
         <v>75.183576388888895</v>
       </c>
-      <c r="H34" s="4">
-        <f t="shared" si="10"/>
+      <c r="H35" s="4">
+        <f>H33*H13</f>
         <v>43.091145833333336</v>
       </c>
-      <c r="I34" s="4">
-        <f t="shared" si="10"/>
+      <c r="I35" s="4">
+        <f>I33*I13</f>
         <v>141.63020833333334</v>
       </c>
-      <c r="J34" s="4">
-        <f t="shared" si="10"/>
+      <c r="J35" s="4">
+        <f>J33*J13</f>
         <v>36.196562499999999</v>
       </c>
-      <c r="K34" s="4">
-        <f t="shared" si="10"/>
+      <c r="K35" s="4">
+        <f>K33*K13</f>
         <v>118.969375</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>33</v>
-      </c>
-      <c r="B36" t="s">
-        <v>34</v>
-      </c>
-      <c r="C36">
-        <v>1000</v>
-      </c>
-      <c r="D36">
-        <v>1000</v>
-      </c>
-      <c r="E36">
-        <v>1000</v>
-      </c>
-      <c r="F36">
-        <v>1000</v>
-      </c>
-      <c r="G36">
-        <v>1000</v>
-      </c>
-      <c r="H36">
-        <v>1000</v>
-      </c>
-      <c r="I36">
-        <v>1000</v>
-      </c>
-      <c r="J36">
-        <v>1000</v>
-      </c>
-      <c r="K36">
-        <v>1000</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B37" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37">
+        <v>1000</v>
+      </c>
+      <c r="D37">
+        <v>1000</v>
+      </c>
+      <c r="E37">
+        <v>1000</v>
+      </c>
+      <c r="F37">
+        <v>1000</v>
+      </c>
+      <c r="G37">
+        <v>1000</v>
+      </c>
+      <c r="H37">
+        <v>1000</v>
+      </c>
+      <c r="I37">
+        <v>1000</v>
+      </c>
+      <c r="J37">
+        <v>1000</v>
+      </c>
+      <c r="K37">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>34</v>
       </c>
-      <c r="C37" s="5">
-        <f t="shared" ref="C37:K37" si="11">C36*(C9/(C9+C10+C11))</f>
+      <c r="B38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" s="5">
+        <f>C37*(C9/(C9+C10+C11))</f>
         <v>444.4444444444444</v>
       </c>
-      <c r="D37" s="5">
-        <f t="shared" si="11"/>
+      <c r="D38" s="5">
+        <f>D37*(D9/(D9+D10+D11))</f>
         <v>409.09090909090912</v>
       </c>
-      <c r="E37" s="5">
-        <f t="shared" si="11"/>
+      <c r="E38" s="5">
+        <f>E37*(E9/(E9+E10+E11))</f>
         <v>409.09090909090912</v>
       </c>
-      <c r="F37" s="5">
-        <f t="shared" si="11"/>
+      <c r="F38" s="5">
+        <f>F37*(F9/(F9+F10+F11))</f>
         <v>409.09090909090912</v>
       </c>
-      <c r="G37" s="5">
-        <f t="shared" si="11"/>
+      <c r="G38" s="5">
+        <f>G37*(G9/(G9+G10+G11))</f>
         <v>409.09090909090912</v>
       </c>
-      <c r="H37" s="5">
-        <f t="shared" si="11"/>
+      <c r="H38" s="5">
+        <f>H37*(H9/(H9+H10+H11))</f>
         <v>409.09090909090912</v>
       </c>
-      <c r="I37" s="5">
-        <f t="shared" si="11"/>
+      <c r="I38" s="5">
+        <f>I37*(I9/(I9+I10+I11))</f>
         <v>409.09090909090912</v>
       </c>
-      <c r="J37" s="5">
-        <f t="shared" si="11"/>
+      <c r="J38" s="5">
+        <f>J37*(J9/(J9+J10+J11))</f>
         <v>406.25</v>
       </c>
-      <c r="K37" s="5">
-        <f t="shared" si="11"/>
+      <c r="K38" s="5">
+        <f>K37*(K9/(K9+K10+K11))</f>
         <v>406.25</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>46</v>
-      </c>
-      <c r="B39" t="s">
-        <v>23</v>
-      </c>
-      <c r="C39" s="4">
-        <f t="shared" ref="C39:K39" si="12">C20/C21</f>
-        <v>1.2829324169530354</v>
-      </c>
-      <c r="D39" s="4">
-        <f t="shared" si="12"/>
-        <v>1.285892634207241</v>
-      </c>
-      <c r="E39" s="4">
-        <f t="shared" si="12"/>
-        <v>1.2636363636363637</v>
-      </c>
-      <c r="F39" s="4">
-        <f t="shared" si="12"/>
-        <v>1.3804878048780487</v>
-      </c>
-      <c r="G39" s="4">
-        <f t="shared" si="12"/>
-        <v>1.4298401420959148</v>
-      </c>
-      <c r="H39" s="4">
-        <f t="shared" si="12"/>
-        <v>1.3722627737226278</v>
-      </c>
-      <c r="I39" s="4">
-        <f t="shared" si="12"/>
-        <v>1.5092592592592593</v>
-      </c>
-      <c r="J39" s="4">
-        <f t="shared" si="12"/>
-        <v>1.282258064516129</v>
-      </c>
-      <c r="K39" s="4">
-        <f t="shared" si="12"/>
-        <v>1.3762376237623763</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B40" t="s">
         <v>23</v>
       </c>
       <c r="C40" s="4">
-        <f>LN(C39)</f>
+        <f>C20/C21</f>
+        <v>1.2829324169530354</v>
+      </c>
+      <c r="D40" s="4">
+        <f>D20/D21</f>
+        <v>1.285892634207241</v>
+      </c>
+      <c r="E40" s="4">
+        <f>E20/E21</f>
+        <v>1.2636363636363637</v>
+      </c>
+      <c r="F40" s="4">
+        <f>F20/F21</f>
+        <v>1.3804878048780487</v>
+      </c>
+      <c r="G40" s="4">
+        <f>G20/G21</f>
+        <v>1.4298401420959148</v>
+      </c>
+      <c r="H40" s="4">
+        <f>H20/H21</f>
+        <v>1.3722627737226278</v>
+      </c>
+      <c r="I40" s="4">
+        <f>I20/I21</f>
+        <v>1.5092592592592593</v>
+      </c>
+      <c r="J40" s="4">
+        <f>J20/J21</f>
+        <v>1.282258064516129</v>
+      </c>
+      <c r="K40" s="4">
+        <f>K20/K21</f>
+        <v>1.3762376237623763</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" t="s">
+        <v>23</v>
+      </c>
+      <c r="C41" s="4">
+        <f>LN(C40)</f>
         <v>0.24914840844953792</v>
       </c>
-      <c r="D40" s="4">
-        <f t="shared" ref="D40:K40" si="13">LN(D39)</f>
+      <c r="D41" s="4">
+        <f t="shared" ref="D41:K41" si="10">LN(D40)</f>
         <v>0.25145313415532228</v>
       </c>
-      <c r="E40" s="4">
-        <f t="shared" si="13"/>
+      <c r="E41" s="4">
+        <f t="shared" si="10"/>
         <v>0.23399356733827556</v>
       </c>
-      <c r="F40" s="4">
-        <f t="shared" si="13"/>
+      <c r="F41" s="4">
+        <f t="shared" si="10"/>
         <v>0.32243691850482936</v>
       </c>
-      <c r="G40" s="4">
-        <f t="shared" si="13"/>
+      <c r="G41" s="4">
+        <f t="shared" si="10"/>
         <v>0.35756264927887305</v>
       </c>
-      <c r="H40" s="4">
-        <f t="shared" si="13"/>
+      <c r="H41" s="4">
+        <f t="shared" si="10"/>
         <v>0.31646103700182437</v>
       </c>
-      <c r="I40" s="4">
-        <f t="shared" si="13"/>
+      <c r="I41" s="4">
+        <f t="shared" si="10"/>
         <v>0.41161897368254269</v>
       </c>
-      <c r="J40" s="4">
-        <f t="shared" si="13"/>
+      <c r="J41" s="4">
+        <f t="shared" si="10"/>
         <v>0.24862263661519463</v>
       </c>
-      <c r="K40" s="4">
-        <f t="shared" si="13"/>
+      <c r="K41" s="4">
+        <f t="shared" si="10"/>
         <v>0.31935341628943237</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>48</v>
-      </c>
-      <c r="B42" t="s">
-        <v>50</v>
-      </c>
-      <c r="C42">
-        <v>2200</v>
-      </c>
-      <c r="D42">
-        <v>2200</v>
-      </c>
-      <c r="E42">
-        <v>2200</v>
-      </c>
-      <c r="F42">
-        <v>2200</v>
-      </c>
-      <c r="G42">
-        <v>2200</v>
-      </c>
-      <c r="H42">
-        <v>2200</v>
-      </c>
-      <c r="I42">
-        <v>2200</v>
-      </c>
-      <c r="J42">
-        <v>2200</v>
-      </c>
-      <c r="K42">
-        <v>2200</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>47</v>
+      </c>
+      <c r="B43" t="s">
         <v>49</v>
       </c>
-      <c r="B43" t="s">
-        <v>50</v>
-      </c>
-      <c r="C43" s="5">
-        <f>C40*C42</f>
-        <v>548.1264985889834</v>
-      </c>
-      <c r="D43" s="5">
-        <f t="shared" ref="D43:K43" si="14">D40*D42</f>
-        <v>553.19689514170898</v>
-      </c>
-      <c r="E43" s="5">
-        <f t="shared" si="14"/>
-        <v>514.78584814420628</v>
-      </c>
-      <c r="F43" s="5">
-        <f t="shared" si="14"/>
-        <v>709.36122071062459</v>
-      </c>
-      <c r="G43" s="10">
-        <f t="shared" si="14"/>
-        <v>786.63782841352065</v>
-      </c>
-      <c r="H43" s="5">
-        <f t="shared" si="14"/>
-        <v>696.2142814040136</v>
-      </c>
-      <c r="I43" s="5">
-        <f t="shared" si="14"/>
-        <v>905.56174210159395</v>
-      </c>
-      <c r="J43" s="5">
-        <f t="shared" si="14"/>
-        <v>546.96980055342817</v>
-      </c>
-      <c r="K43" s="5">
-        <f t="shared" si="14"/>
-        <v>702.57751583675122</v>
+      <c r="C43">
+        <v>2200</v>
+      </c>
+      <c r="D43">
+        <v>2200</v>
+      </c>
+      <c r="E43">
+        <v>2200</v>
+      </c>
+      <c r="F43">
+        <v>2200</v>
+      </c>
+      <c r="G43">
+        <v>2200</v>
+      </c>
+      <c r="H43">
+        <v>2200</v>
+      </c>
+      <c r="I43">
+        <v>2200</v>
+      </c>
+      <c r="J43">
+        <v>2200</v>
+      </c>
+      <c r="K43">
+        <v>2200</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>48</v>
+      </c>
+      <c r="B44" t="s">
+        <v>49</v>
+      </c>
+      <c r="C44" s="5">
+        <f>C41*C43</f>
+        <v>548.1264985889834</v>
+      </c>
+      <c r="D44" s="5">
+        <f t="shared" ref="D44:K44" si="11">D41*D43</f>
+        <v>553.19689514170898</v>
+      </c>
+      <c r="E44" s="5">
+        <f t="shared" si="11"/>
+        <v>514.78584814420628</v>
+      </c>
+      <c r="F44" s="5">
+        <f t="shared" si="11"/>
+        <v>709.36122071062459</v>
+      </c>
+      <c r="G44" s="10">
+        <f t="shared" si="11"/>
+        <v>786.63782841352065</v>
+      </c>
+      <c r="H44" s="5">
+        <f t="shared" si="11"/>
+        <v>696.2142814040136</v>
+      </c>
+      <c r="I44" s="5">
+        <f t="shared" si="11"/>
+        <v>905.56174210159395</v>
+      </c>
+      <c r="J44" s="5">
+        <f t="shared" si="11"/>
+        <v>546.96980055342817</v>
+      </c>
+      <c r="K44" s="5">
+        <f t="shared" si="11"/>
+        <v>702.57751583675122</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" t="s">
         <v>51</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C45" s="6">
+        <f>C44/C35</f>
+        <v>10.157897514882071</v>
+      </c>
+      <c r="D45" s="6">
+        <f t="shared" ref="D45:K45" si="12">D44/D35</f>
+        <v>11.695786525739292</v>
+      </c>
+      <c r="E45" s="7">
+        <f t="shared" si="12"/>
+        <v>18.267070930353619</v>
+      </c>
+      <c r="F45" s="6">
+        <f t="shared" si="12"/>
+        <v>7.1702190263565901</v>
+      </c>
+      <c r="G45" s="6">
+        <f t="shared" si="12"/>
+        <v>10.46289450696808</v>
+      </c>
+      <c r="H45" s="6">
+        <f t="shared" si="12"/>
+        <v>16.156782743647863</v>
+      </c>
+      <c r="I45" s="6">
+        <f t="shared" si="12"/>
+        <v>6.3938460075573138</v>
+      </c>
+      <c r="J45" s="6">
+        <f t="shared" si="12"/>
+        <v>15.111097926866071</v>
+      </c>
+      <c r="K45" s="6">
+        <f t="shared" si="12"/>
+        <v>5.9055325442934468</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>52</v>
       </c>
-      <c r="C44" s="6">
-        <f>C43/C34</f>
-        <v>10.157897514882071</v>
-      </c>
-      <c r="D44" s="6">
-        <f t="shared" ref="D44:K44" si="15">D43/D34</f>
-        <v>11.695786525739292</v>
-      </c>
-      <c r="E44" s="7">
-        <f t="shared" si="15"/>
-        <v>18.267070930353619</v>
-      </c>
-      <c r="F44" s="6">
-        <f t="shared" si="15"/>
-        <v>7.1702190263565901</v>
-      </c>
-      <c r="G44" s="6">
-        <f t="shared" si="15"/>
-        <v>10.46289450696808</v>
-      </c>
-      <c r="H44" s="6">
-        <f t="shared" si="15"/>
-        <v>16.156782743647863</v>
-      </c>
-      <c r="I44" s="6">
-        <f t="shared" si="15"/>
-        <v>6.3938460075573138</v>
-      </c>
-      <c r="J44" s="6">
-        <f t="shared" si="15"/>
-        <v>15.111097926866071</v>
-      </c>
-      <c r="K44" s="6">
-        <f t="shared" si="15"/>
-        <v>5.9055325442934468</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="B48" t="s">
+        <v>33</v>
+      </c>
+      <c r="C48">
+        <f>C37*(C2/2)/C3</f>
+        <v>8000</v>
+      </c>
+      <c r="D48">
+        <f>D37*(D2/2)/D3</f>
+        <v>8000</v>
+      </c>
+      <c r="E48">
+        <f>E37*(E2/2)/E3</f>
+        <v>7711.0389610389611</v>
+      </c>
+      <c r="F48">
+        <f>F37*(F2/2)/F3</f>
+        <v>15384.615384615385</v>
+      </c>
+      <c r="G48">
+        <f>G37*(G2/2)/G3</f>
+        <v>20408.163265306121</v>
+      </c>
+      <c r="H48">
+        <f>H37*(H2/2)/H3</f>
+        <v>12000</v>
+      </c>
+      <c r="I48">
+        <f>I37*(I2/2)/I3</f>
+        <v>23076.923076923074</v>
+      </c>
+      <c r="J48">
+        <f>J37*(J2/2)/J3</f>
+        <v>12000</v>
+      </c>
+      <c r="K48">
+        <f>K37*(K2/2)/K3</f>
+        <v>23076.923076923074</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="B49" t="s">
+        <v>33</v>
+      </c>
+      <c r="C49">
+        <f>C48/2</f>
+        <v>4000</v>
+      </c>
+      <c r="D49">
+        <f t="shared" ref="D49:K49" si="13">D48/2</f>
+        <v>4000</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="13"/>
+        <v>3855.5194805194806</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="13"/>
+        <v>7692.3076923076924</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="13"/>
+        <v>10204.08163265306</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="13"/>
+        <v>6000</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="13"/>
+        <v>11538.461538461537</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="13"/>
+        <v>6000</v>
+      </c>
+      <c r="K49">
+        <f t="shared" si="13"/>
+        <v>11538.461538461537</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="B51" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+      <c r="B52" t="s">
+        <v>33</v>
+      </c>
+      <c r="M52" s="3">
+        <v>3.7509238730000001E-4</v>
+      </c>
+      <c r="N52" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M53" s="3">
+        <v>6.2000371819999995E-4</v>
+      </c>
+      <c r="N53">
+        <f>M53/M52</f>
+        <v>1.6529360210771731</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>58</v>
+      </c>
+      <c r="B54" t="s">
+        <v>33</v>
+      </c>
+      <c r="C54">
+        <v>35000</v>
+      </c>
+      <c r="D54">
+        <v>35000</v>
+      </c>
+      <c r="E54">
+        <v>35000</v>
+      </c>
+      <c r="F54">
+        <v>35000</v>
+      </c>
+      <c r="G54">
+        <v>35000</v>
+      </c>
+      <c r="H54">
+        <v>35000</v>
+      </c>
+      <c r="I54">
+        <v>35000</v>
+      </c>
+      <c r="J54">
+        <v>35000</v>
+      </c>
+      <c r="K54">
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L51" s="3">
-        <v>3.7509238730000001E-4</v>
-      </c>
-      <c r="M51" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>57</v>
-      </c>
-      <c r="L52" s="3">
-        <v>6.2000371819999995E-4</v>
-      </c>
-      <c r="M52">
-        <f>L52/L51</f>
-        <v>1.6529360210771731</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N54">
-        <f>7*M52</f>
+      <c r="B55" t="s">
+        <v>23</v>
+      </c>
+      <c r="O55">
+        <f>7*N53</f>
         <v>11.570552147540212</v>
       </c>
     </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C44:K44">
+  <conditionalFormatting sqref="C45:K45">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -1919,7 +2070,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C43:K43">
+  <conditionalFormatting sqref="C44:K44">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1931,7 +2082,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C34:K34">
+  <conditionalFormatting sqref="C35:K35">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
matlab blowdown model wip
</commit_message>
<xml_diff>
--- a/vehicle-sims/thickness-weight-study/matrix.xlsx
+++ b/vehicle-sims/thickness-weight-study/matrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_repos\upstream-salmon-rocket\vehicle-sims\thickness-weight-study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E5A108D-734E-4FB0-A017-DFB71E0BCF7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C94E97-FFAD-416A-9D06-41A6139F41C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="17355" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2573" yWindow="2573" windowWidth="21600" windowHeight="11535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -597,20 +597,20 @@
   <dimension ref="A1:O57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="4" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.86328125" customWidth="1"/>
+    <col min="4" max="5" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>14</v>
       </c>
@@ -636,7 +636,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -671,7 +671,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -706,7 +706,7 @@
         <v>6.5000000000000002E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -750,17 +750,17 @@
         <v>2.87</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1"/>
       <c r="G6" s="11"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -795,7 +795,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -830,7 +830,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -865,7 +865,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -900,7 +900,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -935,7 +935,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -970,7 +970,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1014,7 +1014,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>7.6999999999999999E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>1.1399999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -1119,12 +1119,12 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A20" s="8" t="s">
         <v>24</v>
       </c>
@@ -1159,7 +1159,7 @@
         <v>13.9</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>25</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
         <v>26</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
         <v>18</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
         <v>19</v>
       </c>
@@ -1317,7 +1317,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" s="2" t="s">
         <v>20</v>
       </c>
@@ -1352,7 +1352,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" s="2" t="s">
         <v>44</v>
       </c>
@@ -1396,10 +1396,10 @@
         <v>3.8000000000000007</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" s="2"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>21</v>
       </c>
@@ -1443,15 +1443,15 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" s="2"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>0.96699999999999997</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>59</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>1.8884027777777779</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>60</v>
       </c>
@@ -1547,7 +1547,7 @@
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -1555,43 +1555,43 @@
         <v>28</v>
       </c>
       <c r="C35" s="4">
-        <f>C33*C13</f>
+        <f t="shared" ref="C35:K35" si="10">C33*C13</f>
         <v>53.960625</v>
       </c>
       <c r="D35" s="4">
-        <f>D33*D13</f>
+        <f t="shared" si="10"/>
         <v>47.298819444444447</v>
       </c>
       <c r="E35" s="4">
-        <f>E33*E13</f>
+        <f t="shared" si="10"/>
         <v>28.181083333333337</v>
       </c>
       <c r="F35" s="4">
-        <f>F33*F13</f>
+        <f t="shared" si="10"/>
         <v>98.931597222222223</v>
       </c>
       <c r="G35" s="4">
-        <f>G33*G13</f>
+        <f t="shared" si="10"/>
         <v>75.183576388888895</v>
       </c>
       <c r="H35" s="4">
-        <f>H33*H13</f>
+        <f t="shared" si="10"/>
         <v>43.091145833333336</v>
       </c>
       <c r="I35" s="4">
-        <f>I33*I13</f>
+        <f t="shared" si="10"/>
         <v>141.63020833333334</v>
       </c>
       <c r="J35" s="4">
-        <f>J33*J13</f>
+        <f t="shared" si="10"/>
         <v>36.196562499999999</v>
       </c>
       <c r="K35" s="4">
-        <f>K33*K13</f>
+        <f t="shared" si="10"/>
         <v>118.969375</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>32</v>
       </c>
@@ -1626,7 +1626,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>34</v>
       </c>
@@ -1634,43 +1634,43 @@
         <v>33</v>
       </c>
       <c r="C38" s="5">
-        <f>C37*(C9/(C9+C10+C11))</f>
+        <f t="shared" ref="C38:K38" si="11">C37*(C9/(C9+C10+C11))</f>
         <v>444.4444444444444</v>
       </c>
       <c r="D38" s="5">
-        <f>D37*(D9/(D9+D10+D11))</f>
+        <f t="shared" si="11"/>
         <v>409.09090909090912</v>
       </c>
       <c r="E38" s="5">
-        <f>E37*(E9/(E9+E10+E11))</f>
+        <f t="shared" si="11"/>
         <v>409.09090909090912</v>
       </c>
       <c r="F38" s="5">
-        <f>F37*(F9/(F9+F10+F11))</f>
+        <f t="shared" si="11"/>
         <v>409.09090909090912</v>
       </c>
       <c r="G38" s="5">
-        <f>G37*(G9/(G9+G10+G11))</f>
+        <f t="shared" si="11"/>
         <v>409.09090909090912</v>
       </c>
       <c r="H38" s="5">
-        <f>H37*(H9/(H9+H10+H11))</f>
+        <f t="shared" si="11"/>
         <v>409.09090909090912</v>
       </c>
       <c r="I38" s="5">
-        <f>I37*(I9/(I9+I10+I11))</f>
+        <f t="shared" si="11"/>
         <v>409.09090909090912</v>
       </c>
       <c r="J38" s="5">
-        <f>J37*(J9/(J9+J10+J11))</f>
+        <f t="shared" si="11"/>
         <v>406.25</v>
       </c>
       <c r="K38" s="5">
-        <f>K37*(K9/(K9+K10+K11))</f>
+        <f t="shared" si="11"/>
         <v>406.25</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>45</v>
       </c>
@@ -1678,43 +1678,43 @@
         <v>23</v>
       </c>
       <c r="C40" s="4">
-        <f>C20/C21</f>
+        <f t="shared" ref="C40:K40" si="12">C20/C21</f>
         <v>1.2829324169530354</v>
       </c>
       <c r="D40" s="4">
-        <f>D20/D21</f>
+        <f t="shared" si="12"/>
         <v>1.285892634207241</v>
       </c>
       <c r="E40" s="4">
-        <f>E20/E21</f>
+        <f t="shared" si="12"/>
         <v>1.2636363636363637</v>
       </c>
       <c r="F40" s="4">
-        <f>F20/F21</f>
+        <f t="shared" si="12"/>
         <v>1.3804878048780487</v>
       </c>
       <c r="G40" s="4">
-        <f>G20/G21</f>
+        <f t="shared" si="12"/>
         <v>1.4298401420959148</v>
       </c>
       <c r="H40" s="4">
-        <f>H20/H21</f>
+        <f t="shared" si="12"/>
         <v>1.3722627737226278</v>
       </c>
       <c r="I40" s="4">
-        <f>I20/I21</f>
+        <f t="shared" si="12"/>
         <v>1.5092592592592593</v>
       </c>
       <c r="J40" s="4">
-        <f>J20/J21</f>
+        <f t="shared" si="12"/>
         <v>1.282258064516129</v>
       </c>
       <c r="K40" s="4">
-        <f>K20/K21</f>
+        <f t="shared" si="12"/>
         <v>1.3762376237623763</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>46</v>
       </c>
@@ -1726,39 +1726,39 @@
         <v>0.24914840844953792</v>
       </c>
       <c r="D41" s="4">
-        <f t="shared" ref="D41:K41" si="10">LN(D40)</f>
+        <f t="shared" ref="D41:K41" si="13">LN(D40)</f>
         <v>0.25145313415532228</v>
       </c>
       <c r="E41" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.23399356733827556</v>
       </c>
       <c r="F41" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.32243691850482936</v>
       </c>
       <c r="G41" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.35756264927887305</v>
       </c>
       <c r="H41" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.31646103700182437</v>
       </c>
       <c r="I41" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.41161897368254269</v>
       </c>
       <c r="J41" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.24862263661519463</v>
       </c>
       <c r="K41" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.31935341628943237</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>47</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -1805,39 +1805,39 @@
         <v>548.1264985889834</v>
       </c>
       <c r="D44" s="5">
-        <f t="shared" ref="D44:K44" si="11">D41*D43</f>
+        <f t="shared" ref="D44:K44" si="14">D41*D43</f>
         <v>553.19689514170898</v>
       </c>
       <c r="E44" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>514.78584814420628</v>
       </c>
       <c r="F44" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>709.36122071062459</v>
       </c>
       <c r="G44" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>786.63782841352065</v>
       </c>
       <c r="H44" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>696.2142814040136</v>
       </c>
       <c r="I44" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>905.56174210159395</v>
       </c>
       <c r="J44" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>546.96980055342817</v>
       </c>
       <c r="K44" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>702.57751583675122</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>50</v>
       </c>
@@ -1849,44 +1849,44 @@
         <v>10.157897514882071</v>
       </c>
       <c r="D45" s="6">
-        <f t="shared" ref="D45:K45" si="12">D44/D35</f>
+        <f t="shared" ref="D45:K45" si="15">D44/D35</f>
         <v>11.695786525739292</v>
       </c>
       <c r="E45" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>18.267070930353619</v>
       </c>
       <c r="F45" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>7.1702190263565901</v>
       </c>
       <c r="G45" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>10.46289450696808</v>
       </c>
       <c r="H45" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>16.156782743647863</v>
       </c>
       <c r="I45" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>6.3938460075573138</v>
       </c>
       <c r="J45" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>15.111097926866071</v>
       </c>
       <c r="K45" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>5.9055325442934468</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>52</v>
       </c>
@@ -1894,43 +1894,43 @@
         <v>33</v>
       </c>
       <c r="C48">
-        <f>C37*(C2/2)/C3</f>
+        <f t="shared" ref="C48:K48" si="16">C37*(C2/2)/C3</f>
         <v>8000</v>
       </c>
       <c r="D48">
-        <f>D37*(D2/2)/D3</f>
+        <f t="shared" si="16"/>
         <v>8000</v>
       </c>
       <c r="E48">
-        <f>E37*(E2/2)/E3</f>
+        <f t="shared" si="16"/>
         <v>7711.0389610389611</v>
       </c>
       <c r="F48">
-        <f>F37*(F2/2)/F3</f>
+        <f t="shared" si="16"/>
         <v>15384.615384615385</v>
       </c>
       <c r="G48">
-        <f>G37*(G2/2)/G3</f>
+        <f t="shared" si="16"/>
         <v>20408.163265306121</v>
       </c>
       <c r="H48">
-        <f>H37*(H2/2)/H3</f>
+        <f t="shared" si="16"/>
         <v>12000</v>
       </c>
       <c r="I48">
-        <f>I37*(I2/2)/I3</f>
+        <f t="shared" si="16"/>
         <v>23076.923076923074</v>
       </c>
       <c r="J48">
-        <f>J37*(J2/2)/J3</f>
+        <f t="shared" si="16"/>
         <v>12000</v>
       </c>
       <c r="K48">
-        <f>K37*(K2/2)/K3</f>
+        <f t="shared" si="16"/>
         <v>23076.923076923074</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>53</v>
       </c>
@@ -1942,39 +1942,39 @@
         <v>4000</v>
       </c>
       <c r="D49">
-        <f t="shared" ref="D49:K49" si="13">D48/2</f>
+        <f t="shared" ref="D49:K49" si="17">D48/2</f>
         <v>4000</v>
       </c>
       <c r="E49">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>3855.5194805194806</v>
       </c>
       <c r="F49">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>7692.3076923076924</v>
       </c>
       <c r="G49">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>10204.08163265306</v>
       </c>
       <c r="H49">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>6000</v>
       </c>
       <c r="I49">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>11538.461538461537</v>
       </c>
       <c r="J49">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>6000</v>
       </c>
       <c r="K49">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>11538.461538461537</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A51" t="s">
         <v>54</v>
       </c>
@@ -1982,7 +1982,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A52" t="s">
         <v>55</v>
       </c>
@@ -1996,7 +1996,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="M53" s="3">
         <v>6.2000371819999995E-4</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>1.6529360210771731</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>58</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>56</v>
       </c>
@@ -2052,7 +2052,7 @@
         <v>11.570552147540212</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
first pass flight simulation
</commit_message>
<xml_diff>
--- a/vehicle-sims/thickness-weight-study/matrix.xlsx
+++ b/vehicle-sims/thickness-weight-study/matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_repos\upstream-salmon-rocket\vehicle-sims\thickness-weight-study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C94E97-FFAD-416A-9D06-41A6139F41C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62CAABB5-504D-4C96-8A96-2DABBDC764B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2573" yWindow="2573" windowWidth="21600" windowHeight="11535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5145" yWindow="5700" windowWidth="21600" windowHeight="11535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="63">
   <si>
     <t>Original Size</t>
   </si>
@@ -220,6 +220,9 @@
   </si>
   <si>
     <t>* TYPICAL VALUE, CHECK LOT TENSILE TEST CERTIFICATE</t>
+  </si>
+  <si>
+    <t>kg</t>
   </si>
 </sst>
 </file>
@@ -594,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O57"/>
+  <dimension ref="A1:O58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1364,11 +1367,11 @@
         <v>2.4699999999999989</v>
       </c>
       <c r="D26">
-        <f t="shared" ref="D26:K26" si="8">D20-D21</f>
+        <f>D20-D21</f>
         <v>2.2900000000000009</v>
       </c>
       <c r="E26">
-        <f t="shared" si="8"/>
+        <f>E20-E21</f>
         <v>2.9000000000000004</v>
       </c>
       <c r="F26">
@@ -1380,685 +1383,727 @@
         <v>2.4200000000000008</v>
       </c>
       <c r="H26">
-        <f t="shared" si="8"/>
+        <f>H20-H21</f>
         <v>5.1000000000000014</v>
       </c>
       <c r="I26">
-        <f t="shared" si="8"/>
+        <f>I20-I21</f>
         <v>5.5</v>
       </c>
       <c r="J26">
-        <f t="shared" si="8"/>
+        <f>J20-J21</f>
         <v>3.5</v>
       </c>
       <c r="K26">
-        <f t="shared" si="8"/>
+        <f>K20-K21</f>
         <v>3.8000000000000007</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" s="2"/>
+      <c r="B27" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27">
+        <f>C26*0.453592</f>
+        <v>1.1203722399999996</v>
+      </c>
+      <c r="D27">
+        <f t="shared" ref="D27:K27" si="8">D26*0.453592</f>
+        <v>1.0387256800000004</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="8"/>
+        <v>1.3154168000000002</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="8"/>
+        <v>1.06140528</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="8"/>
+        <v>1.0976926400000004</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="8"/>
+        <v>2.3133192000000005</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="8"/>
+        <v>2.4947559999999998</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="8"/>
+        <v>1.587572</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="8"/>
+        <v>1.7236496000000003</v>
+      </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="2"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A29" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C29" s="1">
         <f>C23*C25</f>
         <v>58.5</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D29" s="1">
         <f>D23*D25</f>
         <v>54</v>
       </c>
-      <c r="E28" s="1">
-        <f t="shared" ref="E28:K28" si="9">E23*E25</f>
+      <c r="E29" s="1">
+        <f>E23*E25</f>
         <v>72</v>
       </c>
-      <c r="F28" s="1">
-        <f t="shared" si="9"/>
+      <c r="F29" s="1">
+        <f>F23*F25</f>
         <v>44.95</v>
       </c>
-      <c r="G28" s="1">
-        <f t="shared" si="9"/>
+      <c r="G29" s="1">
+        <f>G23*G25</f>
         <v>42.75</v>
       </c>
-      <c r="H28" s="1">
-        <f t="shared" si="9"/>
+      <c r="H29" s="1">
+        <f>H23*H25</f>
         <v>96.5</v>
       </c>
-      <c r="I28" s="1">
-        <f t="shared" si="9"/>
+      <c r="I29" s="1">
+        <f>I23*I25</f>
         <v>84</v>
       </c>
-      <c r="J28" s="1">
-        <f t="shared" si="9"/>
+      <c r="J29" s="1">
+        <f>J23*J25</f>
         <v>82</v>
       </c>
-      <c r="K28" s="1">
-        <f t="shared" si="9"/>
+      <c r="K29" s="1">
+        <f>K23*K25</f>
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A29" s="2"/>
-    </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="2"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A31" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A31" s="2" t="s">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>31</v>
       </c>
-      <c r="C31">
+      <c r="C32">
         <v>8.11</v>
       </c>
-      <c r="D31">
+      <c r="D32">
         <v>6.77</v>
       </c>
-      <c r="E31">
+      <c r="E32">
         <v>4.6100000000000003</v>
       </c>
-      <c r="F31">
+      <c r="F32">
         <v>6.19</v>
       </c>
-      <c r="G31">
+      <c r="G32">
         <v>5.633</v>
       </c>
-      <c r="H31">
+      <c r="H32">
         <v>1.75</v>
       </c>
-      <c r="I31">
+      <c r="I32">
         <v>1.6</v>
       </c>
-      <c r="J31">
+      <c r="J32">
         <v>1.22</v>
       </c>
-      <c r="K31">
+      <c r="K32">
         <v>0.96699999999999997</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
         <v>59</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C34" s="4">
         <f>191.86/288</f>
         <v>0.66618055555555555</v>
       </c>
-      <c r="D33" s="4">
+      <c r="D34" s="4">
         <f>191.86/288</f>
         <v>0.66618055555555555</v>
       </c>
-      <c r="E33" s="4">
+      <c r="E34" s="4">
         <f>95.26/240</f>
         <v>0.3969166666666667</v>
       </c>
-      <c r="F33" s="4">
+      <c r="F34" s="4">
         <f>401.3/288</f>
         <v>1.3934027777777778</v>
       </c>
-      <c r="G33" s="4">
+      <c r="G34" s="4">
         <f>304.97/288</f>
         <v>1.0589236111111111</v>
       </c>
-      <c r="H33" s="4">
+      <c r="H34" s="4">
         <f>165.47/288</f>
         <v>0.57454861111111111</v>
       </c>
-      <c r="I33" s="4">
+      <c r="I34" s="4">
         <f>543.86/288</f>
         <v>1.8884027777777779</v>
       </c>
-      <c r="J33" s="4">
+      <c r="J34" s="4">
         <f>165.47/288</f>
         <v>0.57454861111111111</v>
       </c>
-      <c r="K33" s="4">
+      <c r="K34" s="4">
         <f>543.86/288</f>
         <v>1.8884027777777779</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
-        <v>60</v>
-      </c>
-      <c r="B34" t="s">
-        <v>29</v>
-      </c>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
-    </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
         <v>37</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="4">
-        <f t="shared" ref="C35:K35" si="10">C33*C13</f>
+      <c r="C36" s="4">
+        <f>C34*C13</f>
         <v>53.960625</v>
       </c>
-      <c r="D35" s="4">
-        <f t="shared" si="10"/>
+      <c r="D36" s="4">
+        <f>D34*D13</f>
         <v>47.298819444444447</v>
       </c>
-      <c r="E35" s="4">
-        <f t="shared" si="10"/>
+      <c r="E36" s="4">
+        <f>E34*E13</f>
         <v>28.181083333333337</v>
       </c>
-      <c r="F35" s="4">
-        <f t="shared" si="10"/>
+      <c r="F36" s="4">
+        <f>F34*F13</f>
         <v>98.931597222222223</v>
       </c>
-      <c r="G35" s="4">
-        <f t="shared" si="10"/>
+      <c r="G36" s="4">
+        <f>G34*G13</f>
         <v>75.183576388888895</v>
       </c>
-      <c r="H35" s="4">
-        <f t="shared" si="10"/>
+      <c r="H36" s="4">
+        <f>H34*H13</f>
         <v>43.091145833333336</v>
       </c>
-      <c r="I35" s="4">
-        <f t="shared" si="10"/>
+      <c r="I36" s="4">
+        <f>I34*I13</f>
         <v>141.63020833333334</v>
       </c>
-      <c r="J35" s="4">
-        <f t="shared" si="10"/>
+      <c r="J36" s="4">
+        <f>J34*J13</f>
         <v>36.196562499999999</v>
       </c>
-      <c r="K35" s="4">
-        <f t="shared" si="10"/>
+      <c r="K36" s="4">
+        <f>K34*K13</f>
         <v>118.969375</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
-        <v>32</v>
-      </c>
-      <c r="B37" t="s">
-        <v>33</v>
-      </c>
-      <c r="C37">
-        <v>1000</v>
-      </c>
-      <c r="D37">
-        <v>1000</v>
-      </c>
-      <c r="E37">
-        <v>1000</v>
-      </c>
-      <c r="F37">
-        <v>1000</v>
-      </c>
-      <c r="G37">
-        <v>1000</v>
-      </c>
-      <c r="H37">
-        <v>1000</v>
-      </c>
-      <c r="I37">
-        <v>1000</v>
-      </c>
-      <c r="J37">
-        <v>1000</v>
-      </c>
-      <c r="K37">
-        <v>1000</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B38" t="s">
         <v>33</v>
       </c>
-      <c r="C38" s="5">
-        <f t="shared" ref="C38:K38" si="11">C37*(C9/(C9+C10+C11))</f>
+      <c r="C38">
+        <v>1000</v>
+      </c>
+      <c r="D38">
+        <v>1000</v>
+      </c>
+      <c r="E38">
+        <v>1000</v>
+      </c>
+      <c r="F38">
+        <v>1000</v>
+      </c>
+      <c r="G38">
+        <v>1000</v>
+      </c>
+      <c r="H38">
+        <v>1000</v>
+      </c>
+      <c r="I38">
+        <v>1000</v>
+      </c>
+      <c r="J38">
+        <v>1000</v>
+      </c>
+      <c r="K38">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" t="s">
+        <v>33</v>
+      </c>
+      <c r="C39" s="5">
+        <f>C38*(C9/(C9+C10+C11))</f>
         <v>444.4444444444444</v>
       </c>
-      <c r="D38" s="5">
-        <f t="shared" si="11"/>
+      <c r="D39" s="5">
+        <f>D38*(D9/(D9+D10+D11))</f>
         <v>409.09090909090912</v>
       </c>
-      <c r="E38" s="5">
-        <f t="shared" si="11"/>
+      <c r="E39" s="5">
+        <f>E38*(E9/(E9+E10+E11))</f>
         <v>409.09090909090912</v>
       </c>
-      <c r="F38" s="5">
-        <f t="shared" si="11"/>
+      <c r="F39" s="5">
+        <f>F38*(F9/(F9+F10+F11))</f>
         <v>409.09090909090912</v>
       </c>
-      <c r="G38" s="5">
-        <f t="shared" si="11"/>
+      <c r="G39" s="5">
+        <f>G38*(G9/(G9+G10+G11))</f>
         <v>409.09090909090912</v>
       </c>
-      <c r="H38" s="5">
-        <f t="shared" si="11"/>
+      <c r="H39" s="5">
+        <f>H38*(H9/(H9+H10+H11))</f>
         <v>409.09090909090912</v>
       </c>
-      <c r="I38" s="5">
-        <f t="shared" si="11"/>
+      <c r="I39" s="5">
+        <f>I38*(I9/(I9+I10+I11))</f>
         <v>409.09090909090912</v>
       </c>
-      <c r="J38" s="5">
-        <f t="shared" si="11"/>
+      <c r="J39" s="5">
+        <f>J38*(J9/(J9+J10+J11))</f>
         <v>406.25</v>
       </c>
-      <c r="K38" s="5">
-        <f t="shared" si="11"/>
+      <c r="K39" s="5">
+        <f>K38*(K9/(K9+K10+K11))</f>
         <v>406.25</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A40" t="s">
-        <v>45</v>
-      </c>
-      <c r="B40" t="s">
-        <v>23</v>
-      </c>
-      <c r="C40" s="4">
-        <f t="shared" ref="C40:K40" si="12">C20/C21</f>
-        <v>1.2829324169530354</v>
-      </c>
-      <c r="D40" s="4">
-        <f t="shared" si="12"/>
-        <v>1.285892634207241</v>
-      </c>
-      <c r="E40" s="4">
-        <f t="shared" si="12"/>
-        <v>1.2636363636363637</v>
-      </c>
-      <c r="F40" s="4">
-        <f t="shared" si="12"/>
-        <v>1.3804878048780487</v>
-      </c>
-      <c r="G40" s="4">
-        <f t="shared" si="12"/>
-        <v>1.4298401420959148</v>
-      </c>
-      <c r="H40" s="4">
-        <f t="shared" si="12"/>
-        <v>1.3722627737226278</v>
-      </c>
-      <c r="I40" s="4">
-        <f t="shared" si="12"/>
-        <v>1.5092592592592593</v>
-      </c>
-      <c r="J40" s="4">
-        <f t="shared" si="12"/>
-        <v>1.282258064516129</v>
-      </c>
-      <c r="K40" s="4">
-        <f t="shared" si="12"/>
-        <v>1.3762376237623763</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B41" t="s">
         <v>23</v>
       </c>
       <c r="C41" s="4">
-        <f>LN(C40)</f>
+        <f>C20/C21</f>
+        <v>1.2829324169530354</v>
+      </c>
+      <c r="D41" s="4">
+        <f>D20/D21</f>
+        <v>1.285892634207241</v>
+      </c>
+      <c r="E41" s="4">
+        <f>E20/E21</f>
+        <v>1.2636363636363637</v>
+      </c>
+      <c r="F41" s="4">
+        <f>F20/F21</f>
+        <v>1.3804878048780487</v>
+      </c>
+      <c r="G41" s="4">
+        <f>G20/G21</f>
+        <v>1.4298401420959148</v>
+      </c>
+      <c r="H41" s="4">
+        <f>H20/H21</f>
+        <v>1.3722627737226278</v>
+      </c>
+      <c r="I41" s="4">
+        <f>I20/I21</f>
+        <v>1.5092592592592593</v>
+      </c>
+      <c r="J41" s="4">
+        <f>J20/J21</f>
+        <v>1.282258064516129</v>
+      </c>
+      <c r="K41" s="4">
+        <f>K20/K21</f>
+        <v>1.3762376237623763</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>46</v>
+      </c>
+      <c r="B42" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42" s="4">
+        <f>LN(C41)</f>
         <v>0.24914840844953792</v>
       </c>
-      <c r="D41" s="4">
-        <f t="shared" ref="D41:K41" si="13">LN(D40)</f>
+      <c r="D42" s="4">
+        <f t="shared" ref="D42:K42" si="9">LN(D41)</f>
         <v>0.25145313415532228</v>
       </c>
-      <c r="E41" s="4">
-        <f t="shared" si="13"/>
+      <c r="E42" s="4">
+        <f t="shared" si="9"/>
         <v>0.23399356733827556</v>
       </c>
-      <c r="F41" s="4">
-        <f t="shared" si="13"/>
+      <c r="F42" s="4">
+        <f t="shared" si="9"/>
         <v>0.32243691850482936</v>
       </c>
-      <c r="G41" s="4">
-        <f t="shared" si="13"/>
+      <c r="G42" s="4">
+        <f t="shared" si="9"/>
         <v>0.35756264927887305</v>
       </c>
-      <c r="H41" s="4">
-        <f t="shared" si="13"/>
+      <c r="H42" s="4">
+        <f t="shared" si="9"/>
         <v>0.31646103700182437</v>
       </c>
-      <c r="I41" s="4">
-        <f t="shared" si="13"/>
+      <c r="I42" s="4">
+        <f t="shared" si="9"/>
         <v>0.41161897368254269</v>
       </c>
-      <c r="J41" s="4">
-        <f t="shared" si="13"/>
+      <c r="J42" s="4">
+        <f t="shared" si="9"/>
         <v>0.24862263661519463</v>
       </c>
-      <c r="K41" s="4">
-        <f t="shared" si="13"/>
+      <c r="K42" s="4">
+        <f t="shared" si="9"/>
         <v>0.31935341628943237</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
-        <v>47</v>
-      </c>
-      <c r="B43" t="s">
-        <v>49</v>
-      </c>
-      <c r="C43">
-        <v>2200</v>
-      </c>
-      <c r="D43">
-        <v>2200</v>
-      </c>
-      <c r="E43">
-        <v>2200</v>
-      </c>
-      <c r="F43">
-        <v>2200</v>
-      </c>
-      <c r="G43">
-        <v>2200</v>
-      </c>
-      <c r="H43">
-        <v>2200</v>
-      </c>
-      <c r="I43">
-        <v>2200</v>
-      </c>
-      <c r="J43">
-        <v>2200</v>
-      </c>
-      <c r="K43">
-        <v>2200</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B44" t="s">
         <v>49</v>
       </c>
-      <c r="C44" s="5">
-        <f>C41*C43</f>
-        <v>548.1264985889834</v>
-      </c>
-      <c r="D44" s="5">
-        <f t="shared" ref="D44:K44" si="14">D41*D43</f>
-        <v>553.19689514170898</v>
-      </c>
-      <c r="E44" s="5">
-        <f t="shared" si="14"/>
-        <v>514.78584814420628</v>
-      </c>
-      <c r="F44" s="5">
-        <f t="shared" si="14"/>
-        <v>709.36122071062459</v>
-      </c>
-      <c r="G44" s="10">
-        <f t="shared" si="14"/>
-        <v>786.63782841352065</v>
-      </c>
-      <c r="H44" s="5">
-        <f t="shared" si="14"/>
-        <v>696.2142814040136</v>
-      </c>
-      <c r="I44" s="5">
-        <f t="shared" si="14"/>
-        <v>905.56174210159395</v>
-      </c>
-      <c r="J44" s="5">
-        <f t="shared" si="14"/>
-        <v>546.96980055342817</v>
-      </c>
-      <c r="K44" s="5">
-        <f t="shared" si="14"/>
-        <v>702.57751583675122</v>
+      <c r="C44">
+        <v>2200</v>
+      </c>
+      <c r="D44">
+        <v>2200</v>
+      </c>
+      <c r="E44">
+        <v>2200</v>
+      </c>
+      <c r="F44">
+        <v>2200</v>
+      </c>
+      <c r="G44">
+        <v>2200</v>
+      </c>
+      <c r="H44">
+        <v>2200</v>
+      </c>
+      <c r="I44">
+        <v>2200</v>
+      </c>
+      <c r="J44">
+        <v>2200</v>
+      </c>
+      <c r="K44">
+        <v>2200</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" s="5">
+        <f>C42*C44</f>
+        <v>548.1264985889834</v>
+      </c>
+      <c r="D45" s="5">
+        <f t="shared" ref="D45:K45" si="10">D42*D44</f>
+        <v>553.19689514170898</v>
+      </c>
+      <c r="E45" s="5">
+        <f t="shared" si="10"/>
+        <v>514.78584814420628</v>
+      </c>
+      <c r="F45" s="5">
+        <f t="shared" si="10"/>
+        <v>709.36122071062459</v>
+      </c>
+      <c r="G45" s="10">
+        <f t="shared" si="10"/>
+        <v>786.63782841352065</v>
+      </c>
+      <c r="H45" s="5">
+        <f t="shared" si="10"/>
+        <v>696.2142814040136</v>
+      </c>
+      <c r="I45" s="5">
+        <f t="shared" si="10"/>
+        <v>905.56174210159395</v>
+      </c>
+      <c r="J45" s="5">
+        <f t="shared" si="10"/>
+        <v>546.96980055342817</v>
+      </c>
+      <c r="K45" s="5">
+        <f t="shared" si="10"/>
+        <v>702.57751583675122</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
         <v>50</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>51</v>
       </c>
-      <c r="C45" s="6">
-        <f>C44/C35</f>
+      <c r="C46" s="6">
+        <f>C45/C36</f>
         <v>10.157897514882071</v>
       </c>
-      <c r="D45" s="6">
-        <f t="shared" ref="D45:K45" si="15">D44/D35</f>
+      <c r="D46" s="6">
+        <f t="shared" ref="D46:K46" si="11">D45/D36</f>
         <v>11.695786525739292</v>
       </c>
-      <c r="E45" s="7">
-        <f t="shared" si="15"/>
+      <c r="E46" s="7">
+        <f t="shared" si="11"/>
         <v>18.267070930353619</v>
       </c>
-      <c r="F45" s="6">
-        <f t="shared" si="15"/>
+      <c r="F46" s="6">
+        <f t="shared" si="11"/>
         <v>7.1702190263565901</v>
       </c>
-      <c r="G45" s="6">
-        <f t="shared" si="15"/>
+      <c r="G46" s="6">
+        <f t="shared" si="11"/>
         <v>10.46289450696808</v>
       </c>
-      <c r="H45" s="6">
-        <f t="shared" si="15"/>
+      <c r="H46" s="6">
+        <f t="shared" si="11"/>
         <v>16.156782743647863</v>
       </c>
-      <c r="I45" s="6">
-        <f t="shared" si="15"/>
+      <c r="I46" s="6">
+        <f t="shared" si="11"/>
         <v>6.3938460075573138</v>
       </c>
-      <c r="J45" s="6">
-        <f t="shared" si="15"/>
+      <c r="J46" s="6">
+        <f t="shared" si="11"/>
         <v>15.111097926866071</v>
       </c>
-      <c r="K45" s="6">
-        <f t="shared" si="15"/>
+      <c r="K46" s="6">
+        <f t="shared" si="11"/>
         <v>5.9055325442934468</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A47" s="1" t="s">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A48" s="1" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A48" t="s">
-        <v>52</v>
-      </c>
-      <c r="B48" t="s">
-        <v>33</v>
-      </c>
-      <c r="C48">
-        <f t="shared" ref="C48:K48" si="16">C37*(C2/2)/C3</f>
-        <v>8000</v>
-      </c>
-      <c r="D48">
-        <f t="shared" si="16"/>
-        <v>8000</v>
-      </c>
-      <c r="E48">
-        <f t="shared" si="16"/>
-        <v>7711.0389610389611</v>
-      </c>
-      <c r="F48">
-        <f t="shared" si="16"/>
-        <v>15384.615384615385</v>
-      </c>
-      <c r="G48">
-        <f t="shared" si="16"/>
-        <v>20408.163265306121</v>
-      </c>
-      <c r="H48">
-        <f t="shared" si="16"/>
-        <v>12000</v>
-      </c>
-      <c r="I48">
-        <f t="shared" si="16"/>
-        <v>23076.923076923074</v>
-      </c>
-      <c r="J48">
-        <f t="shared" si="16"/>
-        <v>12000</v>
-      </c>
-      <c r="K48">
-        <f t="shared" si="16"/>
-        <v>23076.923076923074</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B49" t="s">
         <v>33</v>
       </c>
       <c r="C49">
-        <f>C48/2</f>
+        <f>C38*(C2/2)/C3</f>
+        <v>8000</v>
+      </c>
+      <c r="D49">
+        <f>D38*(D2/2)/D3</f>
+        <v>8000</v>
+      </c>
+      <c r="E49">
+        <f>E38*(E2/2)/E3</f>
+        <v>7711.0389610389611</v>
+      </c>
+      <c r="F49">
+        <f>F38*(F2/2)/F3</f>
+        <v>15384.615384615385</v>
+      </c>
+      <c r="G49">
+        <f>G38*(G2/2)/G3</f>
+        <v>20408.163265306121</v>
+      </c>
+      <c r="H49">
+        <f>H38*(H2/2)/H3</f>
+        <v>12000</v>
+      </c>
+      <c r="I49">
+        <f>I38*(I2/2)/I3</f>
+        <v>23076.923076923074</v>
+      </c>
+      <c r="J49">
+        <f>J38*(J2/2)/J3</f>
+        <v>12000</v>
+      </c>
+      <c r="K49">
+        <f>K38*(K2/2)/K3</f>
+        <v>23076.923076923074</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A50" t="s">
+        <v>53</v>
+      </c>
+      <c r="B50" t="s">
+        <v>33</v>
+      </c>
+      <c r="C50">
+        <f>C49/2</f>
         <v>4000</v>
       </c>
-      <c r="D49">
-        <f t="shared" ref="D49:K49" si="17">D48/2</f>
+      <c r="D50">
+        <f t="shared" ref="D50:K50" si="12">D49/2</f>
         <v>4000</v>
       </c>
-      <c r="E49">
-        <f t="shared" si="17"/>
+      <c r="E50">
+        <f t="shared" si="12"/>
         <v>3855.5194805194806</v>
       </c>
-      <c r="F49">
-        <f t="shared" si="17"/>
+      <c r="F50">
+        <f t="shared" si="12"/>
         <v>7692.3076923076924</v>
       </c>
-      <c r="G49">
-        <f t="shared" si="17"/>
+      <c r="G50">
+        <f t="shared" si="12"/>
         <v>10204.08163265306</v>
       </c>
-      <c r="H49">
-        <f t="shared" si="17"/>
+      <c r="H50">
+        <f t="shared" si="12"/>
         <v>6000</v>
       </c>
-      <c r="I49">
-        <f t="shared" si="17"/>
+      <c r="I50">
+        <f t="shared" si="12"/>
         <v>11538.461538461537</v>
       </c>
-      <c r="J49">
-        <f t="shared" si="17"/>
+      <c r="J50">
+        <f t="shared" si="12"/>
         <v>6000</v>
       </c>
-      <c r="K49">
-        <f t="shared" si="17"/>
+      <c r="K50">
+        <f t="shared" si="12"/>
         <v>11538.461538461537</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A51" t="s">
-        <v>54</v>
-      </c>
-      <c r="B51" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="52" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A52" t="s">
+        <v>54</v>
+      </c>
+      <c r="B52" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A53" t="s">
         <v>55</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>33</v>
       </c>
-      <c r="M52" s="3">
+      <c r="M53" s="3">
         <v>3.7509238730000001E-4</v>
       </c>
-      <c r="N52" t="s">
+      <c r="N53" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="M53" s="3">
+    <row r="54" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="M54" s="3">
         <v>6.2000371819999995E-4</v>
       </c>
-      <c r="N53">
-        <f>M53/M52</f>
+      <c r="N54">
+        <f>M54/M53</f>
         <v>1.6529360210771731</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A54" t="s">
-        <v>58</v>
-      </c>
-      <c r="B54" t="s">
-        <v>33</v>
-      </c>
-      <c r="C54">
-        <v>35000</v>
-      </c>
-      <c r="D54">
-        <v>35000</v>
-      </c>
-      <c r="E54">
-        <v>35000</v>
-      </c>
-      <c r="F54">
-        <v>35000</v>
-      </c>
-      <c r="G54">
-        <v>35000</v>
-      </c>
-      <c r="H54">
-        <v>35000</v>
-      </c>
-      <c r="I54">
-        <v>35000</v>
-      </c>
-      <c r="J54">
-        <v>35000</v>
-      </c>
-      <c r="K54">
-        <v>35000</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
+        <v>58</v>
+      </c>
+      <c r="B55" t="s">
+        <v>33</v>
+      </c>
+      <c r="C55">
+        <v>35000</v>
+      </c>
+      <c r="D55">
+        <v>35000</v>
+      </c>
+      <c r="E55">
+        <v>35000</v>
+      </c>
+      <c r="F55">
+        <v>35000</v>
+      </c>
+      <c r="G55">
+        <v>35000</v>
+      </c>
+      <c r="H55">
+        <v>35000</v>
+      </c>
+      <c r="I55">
+        <v>35000</v>
+      </c>
+      <c r="J55">
+        <v>35000</v>
+      </c>
+      <c r="K55">
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
         <v>56</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>23</v>
       </c>
-      <c r="O55">
-        <f>7*N53</f>
+      <c r="O56">
+        <f>7*N54</f>
         <v>11.570552147540212</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A57" t="s">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
         <v>61</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C45:K45">
+  <conditionalFormatting sqref="C46:K46">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -2070,7 +2115,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C44:K44">
+  <conditionalFormatting sqref="C45:K45">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2082,7 +2127,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C35:K35">
+  <conditionalFormatting sqref="C36:K36">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -2097,7 +2142,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="I33" formula="1"/>
+    <ignoredError sqref="I34" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
combined loading von Mises on PV complete
</commit_message>
<xml_diff>
--- a/vehicle-sims/thickness-weight-study/matrix.xlsx
+++ b/vehicle-sims/thickness-weight-study/matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_repos\upstream-salmon-rocket\vehicle-sims\thickness-weight-study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62CAABB5-504D-4C96-8A96-2DABBDC764B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B10AAB8-4D5B-4806-92CD-AB0F458640E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5145" yWindow="5700" windowWidth="21600" windowHeight="11535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-10890" yWindow="7920" windowWidth="21600" windowHeight="11535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="67">
   <si>
     <t>Original Size</t>
   </si>
@@ -204,9 +204,6 @@
     <t>von Mises combined stress</t>
   </si>
   <si>
-    <t>FOS</t>
-  </si>
-  <si>
     <t>Thin Wall PV Estimation</t>
   </si>
   <si>
@@ -223,14 +220,30 @@
   </si>
   <si>
     <t>kg</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Cross-section</t>
+  </si>
+  <si>
+    <t>in^2</t>
+  </si>
+  <si>
+    <t>axial aero stress</t>
+  </si>
+  <si>
+    <t>FOS on vMises</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="170" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -302,7 +315,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -317,6 +330,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -597,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O58"/>
+  <dimension ref="A1:O62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -608,9 +622,8 @@
     <col min="1" max="1" width="26.3984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.86328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.86328125" customWidth="1"/>
-    <col min="4" max="5" width="11.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="11" width="10.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.45">
@@ -1363,81 +1376,81 @@
         <v>22</v>
       </c>
       <c r="C26">
-        <f>C20-C21</f>
+        <f t="shared" ref="C26:K26" si="8">C20-C21</f>
         <v>2.4699999999999989</v>
       </c>
       <c r="D26">
-        <f>D20-D21</f>
+        <f t="shared" si="8"/>
         <v>2.2900000000000009</v>
       </c>
       <c r="E26">
-        <f>E20-E21</f>
+        <f t="shared" si="8"/>
         <v>2.9000000000000004</v>
       </c>
       <c r="F26">
-        <f>F20-F21</f>
+        <f t="shared" si="8"/>
         <v>2.34</v>
       </c>
       <c r="G26">
-        <f>G20-G21</f>
+        <f t="shared" si="8"/>
         <v>2.4200000000000008</v>
       </c>
       <c r="H26">
-        <f>H20-H21</f>
+        <f t="shared" si="8"/>
         <v>5.1000000000000014</v>
       </c>
       <c r="I26">
-        <f>I20-I21</f>
+        <f t="shared" si="8"/>
         <v>5.5</v>
       </c>
       <c r="J26">
-        <f>J20-J21</f>
+        <f t="shared" si="8"/>
         <v>3.5</v>
       </c>
       <c r="K26">
-        <f>K20-K21</f>
+        <f t="shared" si="8"/>
         <v>3.8000000000000007</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" s="2"/>
       <c r="B27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C27">
         <f>C26*0.453592</f>
         <v>1.1203722399999996</v>
       </c>
       <c r="D27">
-        <f t="shared" ref="D27:K27" si="8">D26*0.453592</f>
+        <f t="shared" ref="D27:K27" si="9">D26*0.453592</f>
         <v>1.0387256800000004</v>
       </c>
       <c r="E27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.3154168000000002</v>
       </c>
       <c r="F27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.06140528</v>
       </c>
       <c r="G27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.0976926400000004</v>
       </c>
       <c r="H27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2.3133192000000005</v>
       </c>
       <c r="I27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2.4947559999999998</v>
       </c>
       <c r="J27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.587572</v>
       </c>
       <c r="K27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.7236496000000003</v>
       </c>
     </row>
@@ -1452,39 +1465,39 @@
         <v>22</v>
       </c>
       <c r="C29" s="1">
-        <f>C23*C25</f>
+        <f t="shared" ref="C29:K29" si="10">C23*C25</f>
         <v>58.5</v>
       </c>
       <c r="D29" s="1">
-        <f>D23*D25</f>
+        <f t="shared" si="10"/>
         <v>54</v>
       </c>
       <c r="E29" s="1">
-        <f>E23*E25</f>
+        <f t="shared" si="10"/>
         <v>72</v>
       </c>
       <c r="F29" s="1">
-        <f>F23*F25</f>
+        <f t="shared" si="10"/>
         <v>44.95</v>
       </c>
       <c r="G29" s="1">
-        <f>G23*G25</f>
+        <f t="shared" si="10"/>
         <v>42.75</v>
       </c>
       <c r="H29" s="1">
-        <f>H23*H25</f>
+        <f t="shared" si="10"/>
         <v>96.5</v>
       </c>
       <c r="I29" s="1">
-        <f>I23*I25</f>
+        <f t="shared" si="10"/>
         <v>84</v>
       </c>
       <c r="J29" s="1">
-        <f>J23*J25</f>
+        <f t="shared" si="10"/>
         <v>82</v>
       </c>
       <c r="K29" s="1">
-        <f>K23*K25</f>
+        <f t="shared" si="10"/>
         <v>72</v>
       </c>
     </row>
@@ -1533,7 +1546,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B34" t="s">
         <v>29</v>
@@ -1577,7 +1590,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B35" t="s">
         <v>29</v>
@@ -1600,39 +1613,39 @@
         <v>28</v>
       </c>
       <c r="C36" s="4">
-        <f>C34*C13</f>
+        <f t="shared" ref="C36:K36" si="11">C34*C13</f>
         <v>53.960625</v>
       </c>
       <c r="D36" s="4">
-        <f>D34*D13</f>
+        <f t="shared" si="11"/>
         <v>47.298819444444447</v>
       </c>
       <c r="E36" s="4">
-        <f>E34*E13</f>
+        <f t="shared" si="11"/>
         <v>28.181083333333337</v>
       </c>
       <c r="F36" s="4">
-        <f>F34*F13</f>
+        <f t="shared" si="11"/>
         <v>98.931597222222223</v>
       </c>
       <c r="G36" s="4">
-        <f>G34*G13</f>
+        <f t="shared" si="11"/>
         <v>75.183576388888895</v>
       </c>
       <c r="H36" s="4">
-        <f>H34*H13</f>
+        <f t="shared" si="11"/>
         <v>43.091145833333336</v>
       </c>
       <c r="I36" s="4">
-        <f>I34*I13</f>
+        <f t="shared" si="11"/>
         <v>141.63020833333334</v>
       </c>
       <c r="J36" s="4">
-        <f>J34*J13</f>
+        <f t="shared" si="11"/>
         <v>36.196562499999999</v>
       </c>
       <c r="K36" s="4">
-        <f>K34*K13</f>
+        <f t="shared" si="11"/>
         <v>118.969375</v>
       </c>
     </row>
@@ -1679,39 +1692,39 @@
         <v>33</v>
       </c>
       <c r="C39" s="5">
-        <f>C38*(C9/(C9+C10+C11))</f>
+        <f t="shared" ref="C39:K39" si="12">C38*(C9/(C9+C10+C11))</f>
         <v>444.4444444444444</v>
       </c>
       <c r="D39" s="5">
-        <f>D38*(D9/(D9+D10+D11))</f>
+        <f t="shared" si="12"/>
         <v>409.09090909090912</v>
       </c>
       <c r="E39" s="5">
-        <f>E38*(E9/(E9+E10+E11))</f>
+        <f t="shared" si="12"/>
         <v>409.09090909090912</v>
       </c>
       <c r="F39" s="5">
-        <f>F38*(F9/(F9+F10+F11))</f>
+        <f t="shared" si="12"/>
         <v>409.09090909090912</v>
       </c>
       <c r="G39" s="5">
-        <f>G38*(G9/(G9+G10+G11))</f>
+        <f t="shared" si="12"/>
         <v>409.09090909090912</v>
       </c>
       <c r="H39" s="5">
-        <f>H38*(H9/(H9+H10+H11))</f>
+        <f t="shared" si="12"/>
         <v>409.09090909090912</v>
       </c>
       <c r="I39" s="5">
-        <f>I38*(I9/(I9+I10+I11))</f>
+        <f t="shared" si="12"/>
         <v>409.09090909090912</v>
       </c>
       <c r="J39" s="5">
-        <f>J38*(J9/(J9+J10+J11))</f>
+        <f t="shared" si="12"/>
         <v>406.25</v>
       </c>
       <c r="K39" s="5">
-        <f>K38*(K9/(K9+K10+K11))</f>
+        <f t="shared" si="12"/>
         <v>406.25</v>
       </c>
     </row>
@@ -1723,39 +1736,39 @@
         <v>23</v>
       </c>
       <c r="C41" s="4">
-        <f>C20/C21</f>
+        <f t="shared" ref="C41:K41" si="13">C20/C21</f>
         <v>1.2829324169530354</v>
       </c>
       <c r="D41" s="4">
-        <f>D20/D21</f>
+        <f t="shared" si="13"/>
         <v>1.285892634207241</v>
       </c>
       <c r="E41" s="4">
-        <f>E20/E21</f>
+        <f t="shared" si="13"/>
         <v>1.2636363636363637</v>
       </c>
       <c r="F41" s="4">
-        <f>F20/F21</f>
+        <f t="shared" si="13"/>
         <v>1.3804878048780487</v>
       </c>
       <c r="G41" s="4">
-        <f>G20/G21</f>
+        <f t="shared" si="13"/>
         <v>1.4298401420959148</v>
       </c>
       <c r="H41" s="4">
-        <f>H20/H21</f>
+        <f t="shared" si="13"/>
         <v>1.3722627737226278</v>
       </c>
       <c r="I41" s="4">
-        <f>I20/I21</f>
+        <f t="shared" si="13"/>
         <v>1.5092592592592593</v>
       </c>
       <c r="J41" s="4">
-        <f>J20/J21</f>
+        <f t="shared" si="13"/>
         <v>1.282258064516129</v>
       </c>
       <c r="K41" s="4">
-        <f>K20/K21</f>
+        <f t="shared" si="13"/>
         <v>1.3762376237623763</v>
       </c>
     </row>
@@ -1771,35 +1784,35 @@
         <v>0.24914840844953792</v>
       </c>
       <c r="D42" s="4">
-        <f t="shared" ref="D42:K42" si="9">LN(D41)</f>
+        <f t="shared" ref="D42:K42" si="14">LN(D41)</f>
         <v>0.25145313415532228</v>
       </c>
       <c r="E42" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>0.23399356733827556</v>
       </c>
       <c r="F42" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>0.32243691850482936</v>
       </c>
       <c r="G42" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>0.35756264927887305</v>
       </c>
       <c r="H42" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>0.31646103700182437</v>
       </c>
       <c r="I42" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>0.41161897368254269</v>
       </c>
       <c r="J42" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>0.24862263661519463</v>
       </c>
       <c r="K42" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>0.31935341628943237</v>
       </c>
     </row>
@@ -1850,35 +1863,35 @@
         <v>548.1264985889834</v>
       </c>
       <c r="D45" s="5">
-        <f t="shared" ref="D45:K45" si="10">D42*D44</f>
+        <f t="shared" ref="D45:K45" si="15">D42*D44</f>
         <v>553.19689514170898</v>
       </c>
       <c r="E45" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>514.78584814420628</v>
       </c>
       <c r="F45" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>709.36122071062459</v>
       </c>
       <c r="G45" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>786.63782841352065</v>
       </c>
       <c r="H45" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>696.2142814040136</v>
       </c>
       <c r="I45" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>905.56174210159395</v>
       </c>
       <c r="J45" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>546.96980055342817</v>
       </c>
       <c r="K45" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>702.57751583675122</v>
       </c>
     </row>
@@ -1894,41 +1907,41 @@
         <v>10.157897514882071</v>
       </c>
       <c r="D46" s="6">
-        <f t="shared" ref="D46:K46" si="11">D45/D36</f>
+        <f t="shared" ref="D46:K46" si="16">D45/D36</f>
         <v>11.695786525739292</v>
       </c>
       <c r="E46" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>18.267070930353619</v>
       </c>
       <c r="F46" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>7.1702190263565901</v>
       </c>
       <c r="G46" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>10.46289450696808</v>
       </c>
       <c r="H46" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>16.156782743647863</v>
       </c>
       <c r="I46" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>6.3938460075573138</v>
       </c>
       <c r="J46" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>15.111097926866071</v>
       </c>
       <c r="K46" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>5.9055325442934468</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.45">
@@ -1939,39 +1952,39 @@
         <v>33</v>
       </c>
       <c r="C49">
-        <f>C38*(C2/2)/C3</f>
+        <f t="shared" ref="C49:K49" si="17">C38*(C2/2)/C3</f>
         <v>8000</v>
       </c>
       <c r="D49">
-        <f>D38*(D2/2)/D3</f>
+        <f t="shared" si="17"/>
         <v>8000</v>
       </c>
       <c r="E49">
-        <f>E38*(E2/2)/E3</f>
+        <f t="shared" si="17"/>
         <v>7711.0389610389611</v>
       </c>
       <c r="F49">
-        <f>F38*(F2/2)/F3</f>
+        <f t="shared" si="17"/>
         <v>15384.615384615385</v>
       </c>
       <c r="G49">
-        <f>G38*(G2/2)/G3</f>
+        <f t="shared" si="17"/>
         <v>20408.163265306121</v>
       </c>
       <c r="H49">
-        <f>H38*(H2/2)/H3</f>
+        <f t="shared" si="17"/>
         <v>12000</v>
       </c>
       <c r="I49">
-        <f>I38*(I2/2)/I3</f>
+        <f t="shared" si="17"/>
         <v>23076.923076923074</v>
       </c>
       <c r="J49">
-        <f>J38*(J2/2)/J3</f>
+        <f t="shared" si="17"/>
         <v>12000</v>
       </c>
       <c r="K49">
-        <f>K38*(K2/2)/K3</f>
+        <f t="shared" si="17"/>
         <v>23076.923076923074</v>
       </c>
     </row>
@@ -1987,119 +2000,358 @@
         <v>4000</v>
       </c>
       <c r="D50">
-        <f t="shared" ref="D50:K50" si="12">D49/2</f>
+        <f t="shared" ref="D50:K50" si="18">D49/2</f>
         <v>4000</v>
       </c>
       <c r="E50">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>3855.5194805194806</v>
       </c>
       <c r="F50">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>7692.3076923076924</v>
       </c>
       <c r="G50">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>10204.08163265306</v>
       </c>
       <c r="H50">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>6000</v>
       </c>
       <c r="I50">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>11538.461538461537</v>
       </c>
       <c r="J50">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>6000</v>
       </c>
       <c r="K50">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>11538.461538461537</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>54</v>
       </c>
       <c r="B52" t="s">
+        <v>62</v>
+      </c>
+      <c r="C52">
+        <v>100</v>
+      </c>
+      <c r="D52">
+        <v>100</v>
+      </c>
+      <c r="E52">
+        <v>100</v>
+      </c>
+      <c r="F52">
+        <v>100</v>
+      </c>
+      <c r="G52">
+        <v>100</v>
+      </c>
+      <c r="H52">
+        <v>100</v>
+      </c>
+      <c r="I52">
+        <v>100</v>
+      </c>
+      <c r="J52">
+        <v>100</v>
+      </c>
+      <c r="K52">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="B53" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A53" t="s">
-        <v>55</v>
-      </c>
-      <c r="B53" t="s">
-        <v>33</v>
-      </c>
-      <c r="M53" s="3">
-        <v>3.7509238730000001E-4</v>
-      </c>
-      <c r="N53" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="M54" s="3">
-        <v>6.2000371819999995E-4</v>
-      </c>
-      <c r="N54">
-        <f>M54/M53</f>
-        <v>1.6529360210771731</v>
+      <c r="C53" s="6">
+        <f>C52*0.22480894387</f>
+        <v>22.480894386999999</v>
+      </c>
+      <c r="D53" s="6">
+        <f t="shared" ref="D53:K53" si="19">D52*0.22480894387</f>
+        <v>22.480894386999999</v>
+      </c>
+      <c r="E53" s="6">
+        <f t="shared" si="19"/>
+        <v>22.480894386999999</v>
+      </c>
+      <c r="F53" s="6">
+        <f t="shared" si="19"/>
+        <v>22.480894386999999</v>
+      </c>
+      <c r="G53" s="6">
+        <f t="shared" si="19"/>
+        <v>22.480894386999999</v>
+      </c>
+      <c r="H53" s="6">
+        <f t="shared" si="19"/>
+        <v>22.480894386999999</v>
+      </c>
+      <c r="I53" s="6">
+        <f t="shared" si="19"/>
+        <v>22.480894386999999</v>
+      </c>
+      <c r="J53" s="6">
+        <f t="shared" si="19"/>
+        <v>22.480894386999999</v>
+      </c>
+      <c r="K53" s="6">
+        <f t="shared" si="19"/>
+        <v>22.480894386999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A54" t="s">
+        <v>63</v>
+      </c>
+      <c r="B54" t="s">
+        <v>64</v>
+      </c>
+      <c r="C54" s="6">
+        <f>((C2/2)^2*PI())-((C4/2)^2*PI())</f>
+        <v>0.73631077818510793</v>
+      </c>
+      <c r="D54" s="6">
+        <f t="shared" ref="D54:K54" si="20">((D2/2)^2*PI())-((D4/2)^2*PI())</f>
+        <v>0.73631077818510793</v>
+      </c>
+      <c r="E54" s="6">
+        <f t="shared" si="20"/>
+        <v>1.0745315016779302</v>
+      </c>
+      <c r="F54" s="6">
+        <f t="shared" si="20"/>
+        <v>0.39513381600525577</v>
+      </c>
+      <c r="G54" s="6">
+        <f t="shared" si="20"/>
+        <v>0.30033311609053115</v>
+      </c>
+      <c r="H54" s="6">
+        <f t="shared" si="20"/>
+        <v>1.1290098598838316</v>
+      </c>
+      <c r="I54" s="6">
+        <f t="shared" si="20"/>
+        <v>0.59933733848859294</v>
+      </c>
+      <c r="J54" s="6">
+        <f t="shared" si="20"/>
+        <v>1.1290098598838316</v>
+      </c>
+      <c r="K54" s="6">
+        <f t="shared" si="20"/>
+        <v>0.59933733848859294</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="B55" t="s">
         <v>33</v>
       </c>
-      <c r="C55">
+      <c r="C55" s="6">
+        <f>C53/C54</f>
+        <v>30.531801316846025</v>
+      </c>
+      <c r="D55" s="6">
+        <f t="shared" ref="D55:K55" si="21">D53/D54</f>
+        <v>30.531801316846025</v>
+      </c>
+      <c r="E55" s="6">
+        <f t="shared" si="21"/>
+        <v>20.921577777752493</v>
+      </c>
+      <c r="F55" s="6">
+        <f t="shared" si="21"/>
+        <v>56.894382298833605</v>
+      </c>
+      <c r="G55" s="6">
+        <f t="shared" si="21"/>
+        <v>74.853198607054225</v>
+      </c>
+      <c r="H55" s="6">
+        <f t="shared" si="21"/>
+        <v>19.912044337073503</v>
+      </c>
+      <c r="I55" s="6">
+        <f t="shared" si="21"/>
+        <v>37.509584241309327</v>
+      </c>
+      <c r="J55" s="6">
+        <f t="shared" si="21"/>
+        <v>19.912044337073503</v>
+      </c>
+      <c r="K55" s="6">
+        <f t="shared" si="21"/>
+        <v>37.509584241309327</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="6"/>
+      <c r="H56" s="6"/>
+      <c r="I56" s="6"/>
+      <c r="J56" s="6"/>
+      <c r="K56" s="6"/>
+    </row>
+    <row r="57" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A57" t="s">
+        <v>55</v>
+      </c>
+      <c r="B57" t="s">
+        <v>33</v>
+      </c>
+      <c r="C57" s="5">
+        <f>SQRT((C49-(C50+C55))^2+(C50+C55)^2+(-C49)^2)</f>
+        <v>9798.0541120052658</v>
+      </c>
+      <c r="D57" s="5">
+        <f t="shared" ref="D57:K57" si="22">SQRT((D49-(D50+D55))^2+(D50+D55)^2+(-D49)^2)</f>
+        <v>9798.0541120052658</v>
+      </c>
+      <c r="E57" s="5">
+        <f t="shared" si="22"/>
+        <v>9444.1017684491653</v>
+      </c>
+      <c r="F57" s="5">
+        <f t="shared" si="22"/>
+        <v>18842.400583266743</v>
+      </c>
+      <c r="G57" s="5">
+        <f t="shared" si="22"/>
+        <v>24995.017459441166</v>
+      </c>
+      <c r="H57" s="5">
+        <f t="shared" si="22"/>
+        <v>14696.965434368394</v>
+      </c>
+      <c r="I57" s="5">
+        <f t="shared" si="22"/>
+        <v>28263.392966612431</v>
+      </c>
+      <c r="J57" s="5">
+        <f t="shared" si="22"/>
+        <v>14696.965434368394</v>
+      </c>
+      <c r="K57" s="5">
+        <f t="shared" si="22"/>
+        <v>28263.392966612431</v>
+      </c>
+      <c r="M57" s="3">
+        <v>3.7509238730000001E-4</v>
+      </c>
+      <c r="N57" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="M58" s="3">
+        <v>6.2000371819999995E-4</v>
+      </c>
+      <c r="N58">
+        <f>M58/M57</f>
+        <v>1.6529360210771731</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
+        <v>57</v>
+      </c>
+      <c r="B59" t="s">
+        <v>33</v>
+      </c>
+      <c r="C59">
         <v>35000</v>
       </c>
-      <c r="D55">
+      <c r="D59">
         <v>35000</v>
       </c>
-      <c r="E55">
+      <c r="E59">
         <v>35000</v>
       </c>
-      <c r="F55">
+      <c r="F59">
         <v>35000</v>
       </c>
-      <c r="G55">
+      <c r="G59">
         <v>35000</v>
       </c>
-      <c r="H55">
+      <c r="H59">
         <v>35000</v>
       </c>
-      <c r="I55">
+      <c r="I59">
         <v>35000</v>
       </c>
-      <c r="J55">
+      <c r="J59">
         <v>35000</v>
       </c>
-      <c r="K55">
+      <c r="K59">
         <v>35000</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A56" t="s">
-        <v>56</v>
-      </c>
-      <c r="B56" t="s">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
+        <v>66</v>
+      </c>
+      <c r="B60" t="s">
         <v>23</v>
       </c>
-      <c r="O56">
-        <f>7*N54</f>
+      <c r="C60" s="12">
+        <f>C59/C57</f>
+        <v>3.5721378551191645</v>
+      </c>
+      <c r="D60" s="12">
+        <f t="shared" ref="D60:K60" si="23">D59/D57</f>
+        <v>3.5721378551191645</v>
+      </c>
+      <c r="E60" s="12">
+        <f t="shared" si="23"/>
+        <v>3.7060168196119956</v>
+      </c>
+      <c r="F60" s="12">
+        <f t="shared" si="23"/>
+        <v>1.8575127858751841</v>
+      </c>
+      <c r="G60" s="12">
+        <f t="shared" si="23"/>
+        <v>1.4002790778919714</v>
+      </c>
+      <c r="H60" s="12">
+        <f t="shared" si="23"/>
+        <v>2.3814439896656214</v>
+      </c>
+      <c r="I60" s="12">
+        <f t="shared" si="23"/>
+        <v>1.2383509666141475</v>
+      </c>
+      <c r="J60" s="12">
+        <f t="shared" si="23"/>
+        <v>2.3814439896656214</v>
+      </c>
+      <c r="K60" s="12">
+        <f t="shared" si="23"/>
+        <v>1.2383509666141475</v>
+      </c>
+      <c r="O60">
+        <f>7*N58</f>
         <v>11.570552147540212</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A58" t="s">
-        <v>61</v>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A62" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
leak before break satisfied
</commit_message>
<xml_diff>
--- a/vehicle-sims/thickness-weight-study/matrix.xlsx
+++ b/vehicle-sims/thickness-weight-study/matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_repos\upstream-salmon-rocket\vehicle-sims\thickness-weight-study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B10AAB8-4D5B-4806-92CD-AB0F458640E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25BBF12D-515A-452B-A467-2108B0684C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10890" yWindow="7920" windowWidth="21600" windowHeight="11535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5145" yWindow="5700" windowWidth="21600" windowHeight="11535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="72">
   <si>
     <t>Original Size</t>
   </si>
@@ -235,15 +235,31 @@
   </si>
   <si>
     <t>FOS on vMises</t>
+  </si>
+  <si>
+    <t>Leak Before Break</t>
+  </si>
+  <si>
+    <t>6061-T6 Fracture Toughness</t>
+  </si>
+  <si>
+    <t>psi*sqrt(in)</t>
+  </si>
+  <si>
+    <t>Critical crack size</t>
+  </si>
+  <si>
+    <t>FOS Cc vs thickness</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="174" formatCode="0.0000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -315,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -330,7 +346,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -611,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O62"/>
+  <dimension ref="A1:O67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G60" sqref="G60"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="L65" sqref="L65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2352,6 +2369,134 @@
     <row r="62" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A64" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A65" t="s">
+        <v>68</v>
+      </c>
+      <c r="B65" t="s">
+        <v>69</v>
+      </c>
+      <c r="C65">
+        <v>26400</v>
+      </c>
+      <c r="D65">
+        <v>26400</v>
+      </c>
+      <c r="E65">
+        <v>26400</v>
+      </c>
+      <c r="F65">
+        <v>26400</v>
+      </c>
+      <c r="G65">
+        <v>26400</v>
+      </c>
+      <c r="H65">
+        <v>26400</v>
+      </c>
+      <c r="I65">
+        <v>26400</v>
+      </c>
+      <c r="J65">
+        <v>26400</v>
+      </c>
+      <c r="K65">
+        <v>26400</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A66" t="s">
+        <v>70</v>
+      </c>
+      <c r="B66" t="s">
+        <v>15</v>
+      </c>
+      <c r="C66" s="13">
+        <f>(C65/C57)^2/PI()</f>
+        <v>2.3108848948224328</v>
+      </c>
+      <c r="D66" s="13">
+        <f t="shared" ref="D66:K66" si="24">(D65/D57)^2/PI()</f>
+        <v>2.3108848948224328</v>
+      </c>
+      <c r="E66" s="13">
+        <f t="shared" si="24"/>
+        <v>2.4873486504138747</v>
+      </c>
+      <c r="F66" s="13">
+        <f t="shared" si="24"/>
+        <v>0.62486401645212497</v>
+      </c>
+      <c r="G66" s="13">
+        <f t="shared" si="24"/>
+        <v>0.35510034328348755</v>
+      </c>
+      <c r="H66" s="13">
+        <f t="shared" si="24"/>
+        <v>1.0270761288186727</v>
+      </c>
+      <c r="I66" s="13">
+        <f t="shared" si="24"/>
+        <v>0.27772142649234943</v>
+      </c>
+      <c r="J66" s="13">
+        <f t="shared" si="24"/>
+        <v>1.0270761288186727</v>
+      </c>
+      <c r="K66" s="13">
+        <f t="shared" si="24"/>
+        <v>0.27772142649234943</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A67" t="s">
+        <v>71</v>
+      </c>
+      <c r="B67" t="s">
+        <v>23</v>
+      </c>
+      <c r="C67" s="12">
+        <f>C66/C3</f>
+        <v>18.487079158579462</v>
+      </c>
+      <c r="D67" s="12">
+        <f t="shared" ref="D67:K67" si="25">D66/D3</f>
+        <v>18.487079158579462</v>
+      </c>
+      <c r="E67" s="12">
+        <f t="shared" si="25"/>
+        <v>16.151614613077108</v>
+      </c>
+      <c r="F67" s="12">
+        <f t="shared" si="25"/>
+        <v>9.6132925608019217</v>
+      </c>
+      <c r="G67" s="12">
+        <f t="shared" si="25"/>
+        <v>7.2469457812956639</v>
+      </c>
+      <c r="H67" s="12">
+        <f t="shared" si="25"/>
+        <v>8.2166090305493817</v>
+      </c>
+      <c r="I67" s="12">
+        <f t="shared" si="25"/>
+        <v>4.2726373306515297</v>
+      </c>
+      <c r="J67" s="12">
+        <f t="shared" si="25"/>
+        <v>8.2166090305493817</v>
+      </c>
+      <c r="K67" s="12">
+        <f t="shared" si="25"/>
+        <v>4.2726373306515297</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
prelim SW FEA for bolt tearout and stress raisers
</commit_message>
<xml_diff>
--- a/vehicle-sims/thickness-weight-study/matrix.xlsx
+++ b/vehicle-sims/thickness-weight-study/matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_repos\upstream-salmon-rocket\vehicle-sims\thickness-weight-study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25BBF12D-515A-452B-A467-2108B0684C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231739BE-A57C-4DA1-BE55-624A0E00C065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5145" yWindow="5700" windowWidth="21600" windowHeight="11535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -259,7 +259,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="174" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -347,7 +347,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -634,16 +634,16 @@
       <selection activeCell="L65" sqref="L65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.86328125" customWidth="1"/>
-    <col min="4" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="11" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="4" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="11" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>14</v>
       </c>
@@ -669,7 +669,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -704,7 +704,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -739,7 +739,7 @@
         <v>6.5000000000000002E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -783,17 +783,17 @@
         <v>2.87</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1"/>
       <c r="G6" s="11"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -828,7 +828,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -863,7 +863,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -898,7 +898,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -933,7 +933,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -968,7 +968,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1047,7 +1047,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>7.6999999999999999E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1117,7 +1117,7 @@
         <v>1.1399999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -1152,12 +1152,12 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>24</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>13.9</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>25</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>26</v>
       </c>
@@ -1262,7 +1262,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>18</v>
       </c>
@@ -1306,7 +1306,7 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>19</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>20</v>
       </c>
@@ -1385,7 +1385,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>44</v>
       </c>
@@ -1429,7 +1429,7 @@
         <v>3.8000000000000007</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" t="s">
         <v>61</v>
@@ -1471,10 +1471,10 @@
         <v>1.7236496000000003</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>21</v>
       </c>
@@ -1518,15 +1518,15 @@
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
@@ -1561,7 +1561,7 @@
         <v>0.96699999999999997</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>58</v>
       </c>
@@ -1605,7 +1605,7 @@
         <v>1.8884027777777779</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>59</v>
       </c>
@@ -1622,7 +1622,7 @@
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -1666,7 +1666,7 @@
         <v>118.969375</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>32</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>34</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>406.25</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -1789,7 +1789,7 @@
         <v>1.3762376237623763</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -1833,7 +1833,7 @@
         <v>0.31935341628943237</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>47</v>
       </c>
@@ -1868,7 +1868,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>48</v>
       </c>
@@ -1912,7 +1912,7 @@
         <v>702.57751583675122</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>50</v>
       </c>
@@ -1956,12 +1956,12 @@
         <v>5.9055325442934468</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>23076.923076923074</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>53</v>
       </c>
@@ -2049,7 +2049,7 @@
         <v>11538.461538461537</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>54</v>
       </c>
@@ -2084,7 +2084,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>22</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>22.480894386999999</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>63</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>0.59933733848859294</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>65</v>
       </c>
@@ -2213,7 +2213,7 @@
         <v>37.509584241309327</v>
       </c>
     </row>
-    <row r="56" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C56" s="6"/>
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
@@ -2224,7 +2224,7 @@
       <c r="J56" s="6"/>
       <c r="K56" s="6"/>
     </row>
-    <row r="57" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -2274,7 +2274,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="58" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="M58" s="3">
         <v>6.2000371819999995E-4</v>
       </c>
@@ -2283,7 +2283,7 @@
         <v>1.6529360210771731</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -2318,7 +2318,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>66</v>
       </c>
@@ -2366,17 +2366,17 @@
         <v>11.570552147540212</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>68</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>26400</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>70</v>
       </c>
@@ -2455,7 +2455,7 @@
         <v>0.27772142649234943</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>71</v>
       </c>

</xml_diff>

<commit_message>
adding space for burst disks
</commit_message>
<xml_diff>
--- a/vehicle-sims/thickness-weight-study/matrix.xlsx
+++ b/vehicle-sims/thickness-weight-study/matrix.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_repos\upstream-salmon-rocket\vehicle-sims\thickness-weight-study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231739BE-A57C-4DA1-BE55-624A0E00C065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320F44C4-B4B5-4366-B45E-55D2A2F37410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19131" yWindow="11666" windowWidth="9189" windowHeight="4945" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Rocket Sizing" sheetId="1" r:id="rId1"/>
+    <sheet name="Misc Sizing" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="83">
   <si>
     <t>Original Size</t>
   </si>
@@ -250,6 +251,39 @@
   </si>
   <si>
     <t>FOS Cc vs thickness</t>
+  </si>
+  <si>
+    <t>ID\OD</t>
+  </si>
+  <si>
+    <t>Area Ratios in Concentric Tubes</t>
+  </si>
+  <si>
+    <t>Burst Disk Design</t>
+  </si>
+  <si>
+    <t>ORFS ID</t>
+  </si>
+  <si>
+    <t>0.437500in</t>
+  </si>
+  <si>
+    <t>Face OD</t>
+  </si>
+  <si>
+    <t>0.718750in</t>
+  </si>
+  <si>
+    <t>ORFS Thread</t>
+  </si>
+  <si>
+    <t>ORB Thread</t>
+  </si>
+  <si>
+    <t>3/4"-16</t>
+  </si>
+  <si>
+    <t>13/16"-16</t>
   </si>
 </sst>
 </file>
@@ -331,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -348,6 +382,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -630,7 +665,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L65" sqref="L65"/>
     </sheetView>
   </sheetViews>
@@ -2542,4 +2577,189 @@
     <ignoredError sqref="I34" formula="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC9A7DBF-DD94-46E5-930E-19FA5F483502}">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D2" s="7">
+        <f>3/8</f>
+        <v>0.375</v>
+      </c>
+      <c r="E2" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="F2" s="7">
+        <f>3/4</f>
+        <v>0.75</v>
+      </c>
+      <c r="G2" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C3" s="6">
+        <f>((C2/2)^2-($B3/2)^2)/($B3/2)^2</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="6">
+        <f t="shared" ref="D3:G4" si="0">((D2/2)^2-($B3/2)^2)/($B3/2)^2</f>
+        <v>1.25</v>
+      </c>
+      <c r="E3" s="6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F3" s="6">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="G3" s="6">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <f>3/8</f>
+        <v>0.375</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6">
+        <f>((D2/2)^2-($B4/2)^2)/($B4/2)^2</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="6">
+        <f t="shared" ref="E4:G5" si="1">((E2/2)^2-($B4/2)^2)/($B4/2)^2</f>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="F4" s="6">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="G4" s="6">
+        <f t="shared" si="1"/>
+        <v>6.1111111111111107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6">
+        <f>((E2/2)^2-($B5/2)^2)/($B5/2)^2</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="6">
+        <f t="shared" ref="F5:G6" si="2">((F2/2)^2-($B5/2)^2)/($B5/2)^2</f>
+        <v>1.25</v>
+      </c>
+      <c r="G5" s="6">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <f>3/4</f>
+        <v>0.75</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6">
+        <f>((F2/2)^2-($B6/2)^2)/($B6/2)^2</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="6">
+        <f>((G2/2)^2-($B6/2)^2)/($B6/2)^2</f>
+        <v>0.77777777777777779</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
new size and tube config
</commit_message>
<xml_diff>
--- a/vehicle-sims/thickness-weight-study/matrix.xlsx
+++ b/vehicle-sims/thickness-weight-study/matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_repos\upstream-salmon-rocket\vehicle-sims\thickness-weight-study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5FE62D-0EA0-4FCF-A905-C6B2306D3F6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C43312DB-AAC8-46A3-AF93-AD6778CE1FE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="28800" windowHeight="17355" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36450" yWindow="1950" windowWidth="28800" windowHeight="17355" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rocket Sizing" sheetId="1" r:id="rId1"/>
@@ -668,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,7 +681,7 @@
     <col min="6" max="11" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>14</v>
       </c>
@@ -707,7 +707,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -742,7 +742,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -777,7 +777,7 @@
         <v>6.5000000000000002E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -821,17 +821,17 @@
         <v>2.87</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1"/>
       <c r="G6" s="11"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -865,8 +865,12 @@
       <c r="K7">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M7">
+        <f>SUM(G7:G10)</f>
+        <v>43.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -900,8 +904,12 @@
       <c r="K8">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <f>SUM(G11:G12)</f>
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -921,7 +929,8 @@
         <v>18</v>
       </c>
       <c r="G9" s="11">
-        <v>18</v>
+        <f>18*3/4</f>
+        <v>13.5</v>
       </c>
       <c r="H9">
         <v>18</v>
@@ -936,7 +945,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -956,7 +965,8 @@
         <v>16</v>
       </c>
       <c r="G10" s="11">
-        <v>16</v>
+        <f>16*3/4</f>
+        <v>12</v>
       </c>
       <c r="H10">
         <v>16</v>
@@ -971,7 +981,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -991,7 +1001,8 @@
         <v>10</v>
       </c>
       <c r="G11" s="11">
-        <v>10</v>
+        <f>10*3/4</f>
+        <v>7.5</v>
       </c>
       <c r="H11">
         <v>10</v>
@@ -1006,7 +1017,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1041,7 +1052,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1066,7 +1077,7 @@
       </c>
       <c r="G13" s="11">
         <f t="shared" si="3"/>
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="H13">
         <f t="shared" ref="H13" si="4">SUM(H7:H12)</f>
@@ -1085,7 +1096,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1120,7 +1131,7 @@
         <v>7.6999999999999999E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1324,8 +1335,7 @@
         <v>8.99</v>
       </c>
       <c r="G23">
-        <f>G20+G22</f>
-        <v>8.5500000000000007</v>
+        <v>8.5</v>
       </c>
       <c r="H23">
         <f t="shared" si="6"/>
@@ -1537,7 +1547,7 @@
       </c>
       <c r="G29" s="1">
         <f t="shared" si="10"/>
-        <v>42.75</v>
+        <v>42.5</v>
       </c>
       <c r="H29" s="1">
         <f t="shared" si="10"/>
@@ -1685,7 +1695,7 @@
       </c>
       <c r="G36" s="4">
         <f t="shared" si="11"/>
-        <v>75.183576388888895</v>
+        <v>63.535416666666663</v>
       </c>
       <c r="H36" s="4">
         <f t="shared" si="11"/>
@@ -1975,7 +1985,7 @@
       </c>
       <c r="G46" s="6">
         <f t="shared" si="16"/>
-        <v>10.46289450696808</v>
+        <v>12.381091833245563</v>
       </c>
       <c r="H46" s="6">
         <f t="shared" si="16"/>

</xml_diff>